<commit_message>
Final forward optical model with apertures and thickness for mirrors. Removed old design files. Full telescope model independent of the TIM experiment is also included. Added a .gitignore file to prevent tracking Jupyter checkpoints.
</commit_message>
<xml_diff>
--- a/optics_analysis/OpticalSpecifications.xlsx
+++ b/optics_analysis/OpticalSpecifications.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Engineering Services\TIM\tim-inst_modl\optics_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\IODLab\Consulting\TIM\tim-inst_modl\optics_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F76344-5CA1-4A08-BFBF-32177A3E218D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9907E24C-C885-4B3C-9383-85FE5E38D090}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-8790" windowWidth="21840" windowHeight="38040" xr2:uid="{389EF5AB-58B1-4FD0-BB67-880618441655}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="233">
   <si>
     <t>Entrance Pupil Dia. (mm)</t>
   </si>
@@ -689,6 +689,81 @@
   </si>
   <si>
     <t>Beam Spacing On Sky</t>
+  </si>
+  <si>
+    <t>Spectrometer Optimization</t>
+  </si>
+  <si>
+    <t>Wavelength #1</t>
+  </si>
+  <si>
+    <t>Wavelength #2</t>
+  </si>
+  <si>
+    <t>Wavelength #3</t>
+  </si>
+  <si>
+    <t>Wavelength #4</t>
+  </si>
+  <si>
+    <t>Wavelength #5</t>
+  </si>
+  <si>
+    <t>XFIE</t>
+  </si>
+  <si>
+    <t>YFIE #1</t>
+  </si>
+  <si>
+    <t>YFIE #2</t>
+  </si>
+  <si>
+    <t>YFIE #3</t>
+  </si>
+  <si>
+    <t>YFIE #4</t>
+  </si>
+  <si>
+    <t>YFIE #5</t>
+  </si>
+  <si>
+    <t>Distortion W1</t>
+  </si>
+  <si>
+    <t>Distortion W2</t>
+  </si>
+  <si>
+    <t>Distortion W3</t>
+  </si>
+  <si>
+    <t>Distortion W4</t>
+  </si>
+  <si>
+    <t>Distortion W5</t>
+  </si>
+  <si>
+    <t>Distortion Wavelength Ref</t>
+  </si>
+  <si>
+    <t>Distortion F1</t>
+  </si>
+  <si>
+    <t>Distortion F2</t>
+  </si>
+  <si>
+    <t>Distortion F3</t>
+  </si>
+  <si>
+    <t>Distortion F4</t>
+  </si>
+  <si>
+    <t>Distortion F5</t>
+  </si>
+  <si>
+    <t>mm Array for Pointing (MAP)</t>
+  </si>
+  <si>
+    <t>Wavelength (mm)</t>
   </si>
 </sst>
 </file>
@@ -702,7 +777,7 @@
     <numFmt numFmtId="167" formatCode="0.0000"/>
     <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -771,6 +846,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -835,7 +916,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -890,6 +971,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -904,76 +986,6 @@
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
   <dxfs count="30">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1191,6 +1203,76 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1514,10 +1596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D396856-282B-40CF-8DBB-94DCDACCA298}">
-  <dimension ref="A1:G100"/>
+  <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1532,11 +1614,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1578,12 +1660,10 @@
         <v>109</v>
       </c>
       <c r="B5">
-        <f>2*'Telescope Design'!D4</f>
-        <v>530</v>
+        <v>580</v>
       </c>
       <c r="C5">
-        <f>2*'Telescope Design'!D4</f>
-        <v>530</v>
+        <v>580</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>136</v>
@@ -1707,7 +1787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>94</v>
       </c>
@@ -1716,7 +1796,7 @@
         <v>0.12532783116806537</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>207</v>
       </c>
@@ -1727,63 +1807,63 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>112</v>
       </c>
       <c r="B19">
-        <f>DEGREES(B32/2*B12)*B18</f>
-        <v>0.22431297679371728</v>
+        <f>DEGREES(B36/2*B12)*B18</f>
+        <v>0.46409581405596684</v>
       </c>
       <c r="C19">
-        <f>DEGREES(C32/2*C12)*C18</f>
-        <v>0.22476418105738283</v>
+        <f>DEGREES(C36/2*C12)*C18</f>
+        <v>0.46996146948361867</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>116</v>
       </c>
       <c r="B20">
         <f>2*B13*TAN(RADIANS(B19))</f>
-        <v>62.640320034420093</v>
+        <v>129.60283442638672</v>
       </c>
       <c r="C20">
         <f>2*B13*TAN(RADIANS(C19))</f>
-        <v>62.766321969557531</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>131.24094326440141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>131</v>
       </c>
       <c r="B21">
         <f>B20/2</f>
-        <v>31.320160017210046</v>
+        <v>64.801417213193361</v>
       </c>
       <c r="C21">
         <f>C20/2</f>
-        <v>31.383160984778765</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>65.620471632200704</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>110</v>
       </c>
       <c r="B22">
         <f>100*(B5/B9)^2</f>
-        <v>7.0225000000000009</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+        <v>8.41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -1791,7 +1871,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>89</v>
       </c>
@@ -1805,745 +1885,1064 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27">
         <f>B26*B20</f>
-        <v>62.640320034420093</v>
+        <v>129.60283442638672</v>
       </c>
       <c r="C27">
         <f>C26*C20</f>
-        <v>62.766321969557531</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>131.24094326440141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>131</v>
       </c>
       <c r="B28">
         <f>B27/2</f>
-        <v>31.320160017210046</v>
+        <v>64.801417213193361</v>
       </c>
       <c r="C28">
         <f>C27/2</f>
-        <v>31.383160984778765</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+        <v>65.620471632200704</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>232</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32">
+        <f>5/60*SQRT(2)</f>
+        <v>0.11785113019775792</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B34" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C34" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="B32">
-        <v>29</v>
-      </c>
-      <c r="C32">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+      <c r="B36">
+        <v>60</v>
+      </c>
+      <c r="C36">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="B33">
-        <v>72</v>
-      </c>
-      <c r="C33">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="B37">
+        <v>60</v>
+      </c>
+      <c r="C37">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B34">
-        <f>B38/B39</f>
-        <v>0.34881578763539883</v>
-      </c>
-      <c r="C34">
-        <f>C38/C39</f>
-        <v>0.26461887337857848</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
+      <c r="B38">
+        <f>B42/B43</f>
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="C38">
+        <f>C42/C43</f>
+        <v>0.66395280956806957</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B35">
+      <c r="B39">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C35">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
+      <c r="C39">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="B36">
+      <c r="B40">
         <f>SQRT(3)/2</f>
         <v>0.8660254037844386</v>
       </c>
-      <c r="C36">
+      <c r="C40">
         <f>SQRT(3)/2</f>
         <v>0.8660254037844386</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>164</v>
       </c>
-      <c r="B37">
-        <f>B35*B36</f>
+      <c r="B41">
+        <f>B39*B40</f>
         <v>1.9918584287042087</v>
       </c>
-      <c r="C37">
-        <f>C35*C36</f>
-        <v>1.9918584287042087</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="C41">
+        <f>C39*C40</f>
+        <v>2.1650635094610964</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B38">
-        <f>B35*B32*B36</f>
-        <v>57.763894432422042</v>
-      </c>
-      <c r="C38">
-        <f>C35*C32*C36</f>
-        <v>43.820885431492592</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="B42">
+        <f>B39*B36*B40</f>
+        <v>119.51150572225252</v>
+      </c>
+      <c r="C42">
+        <f>C39*C36*C40</f>
+        <v>99.592921435210442</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B39">
-        <f>B35*B33</f>
-        <v>165.6</v>
-      </c>
-      <c r="C39">
-        <f>C35*C33</f>
-        <v>165.6</v>
-      </c>
-      <c r="E39" s="7"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="B43">
+        <f>B39*B37</f>
+        <v>138</v>
+      </c>
+      <c r="C43">
+        <f>C39*C37</f>
+        <v>150</v>
+      </c>
+      <c r="E43" s="7"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E40" s="7"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="E44" s="7"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>74</v>
       </c>
-      <c r="B41">
+      <c r="B45">
         <f>B10</f>
         <v>240</v>
       </c>
-      <c r="C41">
+      <c r="C45">
         <f>C10</f>
         <v>317</v>
       </c>
-      <c r="E41" s="7"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="E45" s="7"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>75</v>
       </c>
-      <c r="B42">
+      <c r="B46">
         <f>B11</f>
         <v>317</v>
       </c>
-      <c r="C42">
+      <c r="C46">
         <f>C11</f>
         <v>420</v>
       </c>
-      <c r="E42" s="7"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="E46" s="7"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B43">
-        <f>AVERAGE(B41:B42)</f>
+      <c r="B47">
+        <f>AVERAGE(B45:B46)</f>
         <v>278.5</v>
       </c>
-      <c r="C43">
-        <f>AVERAGE(C41:C42)</f>
+      <c r="C47">
+        <f>AVERAGE(C45:C46)</f>
         <v>368.5</v>
       </c>
-      <c r="E43" s="7"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B44">
-        <f>B42-B41</f>
+      <c r="B48">
+        <f>B46-B45</f>
         <v>77</v>
       </c>
-      <c r="C44">
-        <f>C42-C41</f>
+      <c r="C48">
+        <f>C46-C45</f>
         <v>103</v>
       </c>
-      <c r="E44" s="7"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+      <c r="E48" s="7"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B49" t="s">
         <v>80</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C49" t="s">
         <v>80</v>
       </c>
-      <c r="E45" s="7"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
+      <c r="E49" s="7"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B46">
+      <c r="B50">
         <v>-1</v>
       </c>
-      <c r="C46">
+      <c r="C50">
         <v>-1</v>
       </c>
-      <c r="E46" s="7"/>
-    </row>
-    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="E50" s="7"/>
+    </row>
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>83</v>
       </c>
-      <c r="B47">
-        <f>ABS(B46)*B55*1000*B52</f>
-        <v>422.99575599993886</v>
-      </c>
-      <c r="C47">
-        <f>ABS(C46)*C55*1000*C52</f>
-        <v>405.71872762585247</v>
-      </c>
-      <c r="D47" s="18" t="s">
+      <c r="B51">
+        <f>ABS(B50)*B59*1000*B56</f>
+        <v>347.22921081052687</v>
+      </c>
+      <c r="C51">
+        <f>ABS(C50)*C59*1000*C56</f>
+        <v>349.80265109925188</v>
+      </c>
+      <c r="D51" s="18" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B48">
-        <f>B41/B47</f>
-        <v>0.56738157911928244</v>
-      </c>
-      <c r="C48">
-        <f>C41/C47</f>
-        <v>0.78132947388204499</v>
-      </c>
-      <c r="D48" s="18" t="s">
+      <c r="B52">
+        <f>B45/B51</f>
+        <v>0.69118608840476037</v>
+      </c>
+      <c r="C52">
+        <f>C45/C51</f>
+        <v>0.90622526445648766</v>
+      </c>
+      <c r="D52" s="18" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="B50">
+      <c r="B54">
         <v>1</v>
       </c>
-      <c r="C50">
+      <c r="C54">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="B51">
+      <c r="B55">
         <v>-1</v>
       </c>
-      <c r="C51">
+      <c r="C55">
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="B52">
-        <v>3.0856999999999998E-3</v>
-      </c>
-      <c r="C52">
-        <v>2.4803300000000002E-3</v>
-      </c>
-      <c r="D52" s="18" t="s">
+      <c r="B56">
+        <v>2.99E-3</v>
+      </c>
+      <c r="C56">
+        <v>2.2729999999999998E-3</v>
+      </c>
+      <c r="D56" s="18" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
+    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="B53">
-        <v>135</v>
-      </c>
-      <c r="C53">
-        <v>160</v>
-      </c>
-      <c r="D53" s="18" t="s">
+      <c r="B57">
+        <v>115</v>
+      </c>
+      <c r="C57">
+        <v>152</v>
+      </c>
+      <c r="D57" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="17" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="B54">
-        <v>10</v>
-      </c>
-      <c r="C54">
-        <v>12</v>
-      </c>
-      <c r="D54" s="18" t="s">
+      <c r="B58">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>9</v>
+      </c>
+      <c r="D58" s="18" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>200</v>
       </c>
-      <c r="B55" s="27">
-        <f>B53/COS(RADIANS(B54))</f>
-        <v>137.08259260457558</v>
-      </c>
-      <c r="C55" s="27">
-        <f>C53/COS(RADIANS(C54))</f>
-        <v>163.57449517840467</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
+      <c r="B59" s="27">
+        <f>B57/COS(RADIANS(B58))</f>
+        <v>116.13017083964108</v>
+      </c>
+      <c r="C59" s="27">
+        <f>C57/COS(RADIANS(C58))</f>
+        <v>153.89469911977645</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B56" s="27">
-        <f>DEGREES(ASIN((B$46*B$41*B$52 + B$50*SIN(RADIANS(B$54)))/B$51))</f>
-        <v>34.535713684430064</v>
-      </c>
-      <c r="C56" s="27">
-        <f>DEGREES(ASIN((C46*C41*C52 + C50*SIN(RADIANS(C54)))/C51))</f>
-        <v>35.334778943238227</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
+      <c r="B60" s="27">
+        <f>DEGREES(ASIN((B$50*B$45*B$56 + B$54*SIN(RADIANS(B$58)))/B$55))</f>
+        <v>35.339974995111646</v>
+      </c>
+      <c r="C60" s="27">
+        <f>DEGREES(ASIN((C50*C45*C56 + C54*SIN(RADIANS(C58)))/C55))</f>
+        <v>34.340270482554416</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B57" s="27">
-        <f>DEGREES(ASIN((B$46*B$42*B$52 + B$50*SIN(RADIANS(B$54)))/B$51))</f>
-        <v>53.563801264493286</v>
-      </c>
-      <c r="C57" s="27">
-        <f>DEGREES(ASIN((C$46*C$42*C$52 + C$50*SIN(RADIANS(C$54)))/C$51))</f>
-        <v>56.493884831719861</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+      <c r="B61" s="27">
+        <f>DEGREES(ASIN((B$50*B$46*B$56 + B$54*SIN(RADIANS(B$58)))/B$55))</f>
+        <v>53.964913626392374</v>
+      </c>
+      <c r="C61" s="27">
+        <f>DEGREES(ASIN((C$50*C$46*C$56 + C$54*SIN(RADIANS(C$58)))/C$55))</f>
+        <v>52.960985959097115</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B58" s="27">
-        <f>B53/(2*TAN(ASIN(1/(2*$B16))))</f>
-        <v>535.76464049057972</v>
-      </c>
-      <c r="C58" s="27">
-        <f>C53/(2*TAN(ASIN(1/(2*$B16))))</f>
-        <v>634.98031465550184</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="5" t="s">
+      <c r="B62" s="27">
+        <f>B57/(2*TAN(ASIN(1/(2*$B16))))</f>
+        <v>456.39210115864194</v>
+      </c>
+      <c r="C62" s="27">
+        <f>C57/(2*TAN(ASIN(1/(2*$B16))))</f>
+        <v>603.23129892272675</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B59" s="27">
-        <f>2*B58</f>
-        <v>1071.5292809811594</v>
-      </c>
-      <c r="C59" s="27">
-        <f>2*C58</f>
-        <v>1269.9606293110037</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="5" t="s">
+      <c r="B63" s="27">
+        <f>2*B62</f>
+        <v>912.78420231728387</v>
+      </c>
+      <c r="C63" s="27">
+        <f>2*C62</f>
+        <v>1206.4625978454535</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B60" s="27">
-        <f>DEGREES(ASIN((B46*B42*B52+B50*SIN(RADIANS(B54)))/B51) - ASIN((B46*B41*B52+B50*SIN(RADIANS(B54)))/B51))</f>
-        <v>19.028087580063218</v>
-      </c>
-      <c r="C60" s="27">
-        <f>DEGREES(ASIN((C46*C42*C52+C50*SIN(RADIANS(C54)))/C51) - ASIN((C46*C41*C52+C50*SIN(RADIANS(C54)))/C51))</f>
-        <v>21.159105888481633</v>
-      </c>
-      <c r="D60" s="18" t="s">
+      <c r="B64" s="27">
+        <f>DEGREES(ASIN((B50*B46*B56+B54*SIN(RADIANS(B58)))/B55) - ASIN((B50*B45*B56+B54*SIN(RADIANS(B58)))/B55))</f>
+        <v>18.624938631280724</v>
+      </c>
+      <c r="C64" s="27">
+        <f>DEGREES(ASIN((C50*C46*C56+C54*SIN(RADIANS(C58)))/C55) - ASIN((C50*C45*C56+C54*SIN(RADIANS(C58)))/C55))</f>
+        <v>18.620715476542696</v>
+      </c>
+      <c r="D64" s="18" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B61" s="27">
-        <f>2*DEGREES(ATAN($B$28/B58))</f>
-        <v>6.6912700839527224</v>
-      </c>
-      <c r="C61" s="27">
-        <f>2*DEGREES(ATAN($C$28/C58))</f>
-        <v>5.6589493320255677</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+      <c r="B65" s="27">
+        <f>2*DEGREES(ATAN($B$28/B62))</f>
+        <v>16.162395280139727</v>
+      </c>
+      <c r="C65" s="27">
+        <f>2*DEGREES(ATAN($C$28/C62))</f>
+        <v>12.416630687810692</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B62" s="27">
-        <f>B61/B60</f>
-        <v>0.35165226435911179</v>
-      </c>
-      <c r="C62" s="27">
-        <f>C61/C60</f>
-        <v>0.26744746974899947</v>
-      </c>
-      <c r="D62" s="18" t="s">
+      <c r="B66" s="27">
+        <f>B65/B64</f>
+        <v>0.86778247166918787</v>
+      </c>
+      <c r="C66" s="27">
+        <f>C65/C64</f>
+        <v>0.66681813077765173</v>
+      </c>
+      <c r="D66" s="18" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B63" s="27">
-        <f>B39/(2*TAN(RADIANS(B60/2)))</f>
-        <v>494.04934934542291</v>
-      </c>
-      <c r="C63" s="27">
-        <f>C39/(2*TAN(RADIANS(C60/2)))</f>
-        <v>443.31279338162773</v>
-      </c>
-      <c r="D63" s="18" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B64" s="27">
-        <f>2*B63</f>
-        <v>988.09869869084582</v>
-      </c>
-      <c r="C64" s="27">
-        <f>2*C63</f>
-        <v>886.62558676325546</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="B65" s="27">
-        <f>2*B63*TAN(RADIANS(B61/2))</f>
-        <v>57.763067990931461</v>
-      </c>
-      <c r="C65" s="27">
-        <f>2*C63*TAN(RADIANS(C61/2))</f>
-        <v>43.820434870821529</v>
-      </c>
-      <c r="D65" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B66" s="27">
-        <f>B$63/(B$55*COS(RADIANS(B56)))</f>
-        <v>4.3750244223501324</v>
-      </c>
-      <c r="C66" s="27">
-        <f>C$63/(C$55*COS(RADIANS(C56)))</f>
-        <v>3.3221410536458622</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
-        <v>201</v>
+        <v>114</v>
       </c>
       <c r="B67" s="27">
-        <f>B$63/(B$55*COS(RADIANS(B57)))</f>
-        <v>6.0681281171113861</v>
+        <f>B43/(2*TAN(RADIANS(B64/2)))</f>
+        <v>420.78365183067052</v>
       </c>
       <c r="C67" s="27">
-        <f>C$63/(C$55*COS(RADIANS(C57)))</f>
-        <v>4.9094761710441173</v>
+        <f>C43/(2*TAN(RADIANS(C64/2)))</f>
+        <v>457.47911576035671</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B68" s="27">
-        <f>B63/B53</f>
-        <v>3.6596248099660955</v>
+        <f>2*B67</f>
+        <v>841.56730366134104</v>
       </c>
       <c r="C68" s="27">
-        <f>C63/C53</f>
-        <v>2.7707049586351733</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
-        <v>134</v>
+        <f>2*C67</f>
+        <v>914.95823152071341</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>130</v>
       </c>
       <c r="B69" s="27">
-        <f>B66*B41/1000</f>
-        <v>1.0500058613640317</v>
+        <f>2*B67*TAN(RADIANS(B65/2))</f>
+        <v>119.49101182753482</v>
       </c>
       <c r="C69" s="27">
-        <f>C66*C41/1000</f>
-        <v>1.0531187140057383</v>
+        <f>2*C67*TAN(RADIANS(C65/2))</f>
+        <v>99.530629102593295</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
-        <v>134</v>
+        <v>202</v>
       </c>
       <c r="B70" s="27">
-        <f>B67*B42/1000</f>
-        <v>1.9235966131243094</v>
+        <f>B$67/(B$59*COS(RADIANS(B60)))</f>
+        <v>4.4418624994883098</v>
       </c>
       <c r="C70" s="27">
-        <f>C67*C42/1000</f>
-        <v>2.0619799918385291</v>
-      </c>
-      <c r="D70" s="18" t="s">
-        <v>169</v>
+        <f>C$67/(C$59*COS(RADIANS(C60)))</f>
+        <v>3.6001804382732696</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
-        <v>165</v>
+        <v>201</v>
       </c>
       <c r="B71" s="27">
-        <f>B$35/B69</f>
-        <v>2.1904639627555387</v>
+        <f>B$67/(B$59*COS(RADIANS(B61)))</f>
+        <v>6.1592707432699934</v>
       </c>
       <c r="C71" s="27">
-        <f>C$35/C69</f>
-        <v>2.1839892971339481</v>
-      </c>
-      <c r="D71" s="18" t="s">
-        <v>166</v>
+        <f>C$67/(C$59*COS(RADIANS(C61)))</f>
+        <v>4.9350599148916041</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="B72" s="27">
-        <f>B$35/B70</f>
-        <v>1.1956768816848431</v>
+        <f>B67/B57</f>
+        <v>3.6589882767884392</v>
       </c>
       <c r="C72" s="27">
-        <f>C$35/C70</f>
-        <v>1.1154327438207798</v>
-      </c>
-      <c r="D72" s="18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <f>C67/C57</f>
+        <v>3.0097310247391889</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="B73" s="27">
-        <f>B68*B41/1000</f>
-        <v>0.87830995439186288</v>
+        <f>1.5*B72*B46/1000</f>
+        <v>1.7398489256129031</v>
       </c>
       <c r="C73" s="27">
-        <f>C68*C41/1000</f>
-        <v>0.87831347188734987</v>
-      </c>
-      <c r="D73" s="18" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <f>1.5*C72*C46/1000</f>
+        <v>1.8961305455856889</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B74" s="27">
-        <f>B68*B42/1000</f>
-        <v>1.1601010647592522</v>
+        <f>B70*B45/1000</f>
+        <v>1.0660469998771944</v>
       </c>
       <c r="C74" s="27">
-        <f>C68*C42/1000</f>
-        <v>1.1636960826267728</v>
+        <f>C70*C45/1000</f>
+        <v>1.1412571989326266</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>171</v>
+        <v>134</v>
       </c>
       <c r="B75" s="27">
-        <f>B$37/B73</f>
-        <v>2.2678308708038735</v>
+        <f>B71*B46/1000</f>
+        <v>1.952488825616588</v>
       </c>
       <c r="C75" s="27">
-        <f>C$37/C73</f>
-        <v>2.2678217885284573</v>
+        <f>C71*C46/1000</f>
+        <v>2.0727251642544737</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B76" s="27">
+        <f>B$39/B74</f>
+        <v>2.1575033748652293</v>
+      </c>
+      <c r="C76" s="27">
+        <f>C$39/C74</f>
+        <v>2.1905666858777781</v>
+      </c>
+      <c r="D76" s="18" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B77" s="27">
+        <f>B$39/B75</f>
+        <v>1.17798369436182</v>
+      </c>
+      <c r="C77" s="27">
+        <f>C$39/C75</f>
+        <v>1.2061415778194646</v>
+      </c>
+      <c r="D77" s="18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B78" s="27">
+        <f>B72*B45/1000</f>
+        <v>0.87815718642922536</v>
+      </c>
+      <c r="C78" s="27">
+        <f>C72*C45/1000</f>
+        <v>0.95408473484232281</v>
+      </c>
+      <c r="D78" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B79" s="27">
+        <f>B72*B46/1000</f>
+        <v>1.1598992837419353</v>
+      </c>
+      <c r="C79" s="27">
+        <f>C72*C46/1000</f>
+        <v>1.2640870303904594</v>
+      </c>
+      <c r="D79" s="18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B76" s="27">
-        <f>B$37/B74</f>
-        <v>1.7169697444571912</v>
-      </c>
-      <c r="C76" s="27">
-        <f>C$37/C74</f>
-        <v>1.7116654927702879</v>
-      </c>
-      <c r="D76" s="18" t="s">
+      <c r="B80" s="27">
+        <f>B$41/B78</f>
+        <v>2.2682253923167566</v>
+      </c>
+      <c r="C80" s="27">
+        <f>C$41/C78</f>
+        <v>2.2692570485564958</v>
+      </c>
+      <c r="D80" s="18" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B81" s="27">
+        <f>B$41/B79</f>
+        <v>1.7172684358234116</v>
+      </c>
+      <c r="C81" s="27">
+        <f>C$41/C79</f>
+        <v>1.7127487723628787</v>
+      </c>
+      <c r="D81" s="18" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="5"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="5"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="5"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="5"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="5"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="5"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="5"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="5"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="5"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="5"/>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="5"/>
-    </row>
-    <row r="91" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A91" s="4"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="6"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="6"/>
-    </row>
-    <row r="100" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A100" s="3"/>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B84">
+        <v>240</v>
+      </c>
+      <c r="C84">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B85">
+        <f>B84+19.25</f>
+        <v>259.25</v>
+      </c>
+      <c r="C85">
+        <f>C84+25.75</f>
+        <v>342.75</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B86">
+        <f t="shared" ref="B86:B88" si="0">B85+19.25</f>
+        <v>278.5</v>
+      </c>
+      <c r="C86">
+        <f t="shared" ref="C86:C88" si="1">C85+25.75</f>
+        <v>368.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B87">
+        <f t="shared" si="0"/>
+        <v>297.75</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>394.25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B88">
+        <f t="shared" si="0"/>
+        <v>317</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B89">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="C89">
+        <v>-3.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B91">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="C91">
+        <v>0.23499999999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B92">
+        <f>B91*2</f>
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="C92">
+        <f>C91*2</f>
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B93">
+        <f>B91*-1</f>
+        <v>-0.23200000000000001</v>
+      </c>
+      <c r="C93">
+        <f>C91*-1</f>
+        <v>-0.23499999999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B94">
+        <f>B91*-2</f>
+        <v>-0.46400000000000002</v>
+      </c>
+      <c r="C94">
+        <f>C91*-2</f>
+        <v>-0.47</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B96">
+        <f>ASIN((B$50*B86*B$56+B$54*SIN(RADIANS(B$58)))/B$55)</f>
+        <v>0.76639395374515906</v>
+      </c>
+      <c r="C96">
+        <f>ASIN((C$50*C86*C$56+C$54*SIN(RADIANS(C$58)))/C$55)</f>
+        <v>0.74935412039166005</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B97">
+        <f>B$67 * TAN(ASIN((B$50*B84*B$56 + B$54*SIN(RADIANS(B$58)))/B$55) - B$96)</f>
+        <v>-63.420943595754522</v>
+      </c>
+      <c r="C97">
+        <f>C$67 * TAN(ASIN((C$50*C84*C$56 + C$54*SIN(RADIANS(C$58)))/C$55) - C$96)</f>
+        <v>-69.142766201458457</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B98">
+        <f t="shared" ref="B98:B101" si="2">B$67 * TAN(ASIN((B$50*B85*B$56 + B$54*SIN(RADIANS(B$58)))/B$55) - B$96)</f>
+        <v>-32.511293583485532</v>
+      </c>
+      <c r="C98">
+        <f t="shared" ref="C98:C101" si="3">C$67 * TAN(ASIN((C$50*C85*C$56 + C$54*SIN(RADIANS(C$58)))/C$55) - C$96)</f>
+        <v>-35.40930583094336</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B99">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B100">
+        <f t="shared" si="2"/>
+        <v>35.146063281169006</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="3"/>
+        <v>38.179840778570941</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B101">
+        <f t="shared" si="2"/>
+        <v>74.602781180701911</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="3"/>
+        <v>80.881277122658034</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B103" s="28">
+        <f>B$67 * TAN(B90*$B$13/B$62)</f>
+        <v>0</v>
+      </c>
+      <c r="C103" s="28">
+        <f>C$67 * TAN(C90*$B$13/C$62)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B104" s="28">
+        <f t="shared" ref="B104:C107" si="4">B$67 * TAN(RADIANS(B91*$B$13/B$62))</f>
+        <v>29.916185830804324</v>
+      </c>
+      <c r="C104" s="28">
+        <f t="shared" si="4"/>
+        <v>24.908709991071401</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B105" s="28">
+        <f t="shared" si="4"/>
+        <v>60.136342371383464</v>
+      </c>
+      <c r="C105" s="28">
+        <f t="shared" si="4"/>
+        <v>49.965545731922802</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B106" s="28">
+        <f t="shared" si="4"/>
+        <v>-29.916185830804324</v>
+      </c>
+      <c r="C106" s="28">
+        <f t="shared" si="4"/>
+        <v>-24.908709991071401</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B107" s="28">
+        <f t="shared" si="4"/>
+        <v>-60.136342371383464</v>
+      </c>
+      <c r="C107" s="28">
+        <f t="shared" si="4"/>
+        <v>-49.965545731922802</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="5"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="5"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="5"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="5"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="5"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="5"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="5"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="5"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="5"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="5"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="5"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="5"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="5"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="5"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B62:C62">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="notBetween">
-      <formula>$B$34-0.01*$B$34</formula>
-      <formula>$B$34+0.01*$B$34</formula>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <conditionalFormatting sqref="B66:C66">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="notBetween">
+      <formula>$B$38-0.01*$B$38</formula>
+      <formula>$B$38+0.01*$B$38</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="between">
-      <formula>$B$34-0.01*$B$34</formula>
-      <formula>$B$34+0.01*$B$34</formula>
+    <cfRule type="cellIs" dxfId="28" priority="7" operator="between">
+      <formula>$B$38-0.01*$B$38</formula>
+      <formula>$B$38+0.01*$B$38</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="greaterThan">
       <formula>$B$4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B65">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
-      <formula>$B$38</formula>
+  <conditionalFormatting sqref="B69">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="greaterThan">
+      <formula>$B$42</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
-      <formula>$B$38</formula>
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="lessThan">
+      <formula>$B$42</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
-      <formula>$C$38</formula>
+  <conditionalFormatting sqref="C69">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="lessThan">
+      <formula>$C$42</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
-      <formula>$C$38</formula>
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="greaterThan">
+      <formula>$C$42</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2556,7 +2955,7 @@
   <dimension ref="A2:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2749,11 +3148,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -3803,72 +4202,72 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="29" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="greaterThan">
       <formula>$B$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70">
-    <cfRule type="cellIs" dxfId="28" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="17" operator="lessThan">
       <formula>$B$47</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="18" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="20" priority="18" operator="greaterThanOrEqual">
       <formula>$B$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="cellIs" dxfId="26" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="19" priority="15" operator="greaterThanOrEqual">
       <formula>$C$47</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="lessThan">
       <formula>$C$47</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69">
-    <cfRule type="cellIs" dxfId="24" priority="13" operator="notBetween">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58:C60">
-    <cfRule type="cellIs" dxfId="23" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69">
-    <cfRule type="cellIs" dxfId="22" priority="8" operator="notBetween">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="notBetween">
       <formula>-0.000001</formula>
       <formula>0.000001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="21" operator="greaterThan">
       <formula>$B$38</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="22" operator="lessThanOrEqual">
       <formula>$B$38</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C73">
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="lessThanOrEqual">
       <formula>$C$38</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="greaterThan">
       <formula>$C$38</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B74">
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="lessThanOrEqual">
       <formula>$B$39</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
       <formula>$B$39</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThanOrEqual">
       <formula>$C$39</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
       <formula>$C$39</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3897,11 +4296,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -4859,33 +5258,33 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="B61:C61">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="notBetween">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="notBetween">
       <formula>$B$33-0.01*$B$33</formula>
       <formula>$B$33+0.01*$B$33</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="between">
       <formula>$B$33-0.01*$B$33</formula>
       <formula>$B$33+0.01*$B$33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>$B$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>$B$37</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
       <formula>$B$37</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>$C$37</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>$C$37</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5655,11 +6054,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
@@ -5748,17 +6147,17 @@
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="29"/>
+      <c r="C12" s="30"/>
       <c r="D12">
         <v>1.5</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="F12" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="29"/>
+      <c r="G12" s="30"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">

</xml_diff>

<commit_message>
Updated forward Zemax model to latest design.
</commit_message>
<xml_diff>
--- a/optics_analysis/OpticalSpecifications.xlsx
+++ b/optics_analysis/OpticalSpecifications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\IODLab\Consulting\TIM\tim-inst_modl\optics_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9907E24C-C885-4B3C-9383-85FE5E38D090}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E3A6D4-8701-424B-89A5-CF38C3E80114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-8790" windowWidth="21840" windowHeight="38040" xr2:uid="{389EF5AB-58B1-4FD0-BB67-880618441655}"/>
+    <workbookView xWindow="-21720" yWindow="-8790" windowWidth="21840" windowHeight="38040" activeTab="1" xr2:uid="{389EF5AB-58B1-4FD0-BB67-880618441655}"/>
   </bookViews>
   <sheets>
     <sheet name="Spectrometer Design" sheetId="8" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="Old Calcs" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Telescope Design'!$N$4:$N$7</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Telescope Design'!$N$4:$N$7</definedName>
     <definedName name="solver_adj" localSheetId="2" hidden="1">'F Lambda Specs'!$B$67</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">2</definedName>
@@ -65,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="238">
   <si>
     <t>Entrance Pupil Dia. (mm)</t>
   </si>
@@ -764,6 +766,21 @@
   </si>
   <si>
     <t>Wavelength (mm)</t>
+  </si>
+  <si>
+    <t>Reverse Throughput</t>
+  </si>
+  <si>
+    <t>2.16525 mm</t>
+  </si>
+  <si>
+    <t>Waist:</t>
+  </si>
+  <si>
+    <t>Wavelength</t>
+  </si>
+  <si>
+    <t>278.5 um</t>
   </si>
 </sst>
 </file>
@@ -1299,6 +1316,1051 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Reverse Cassegrain Throughput</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Telescope Design'!$L$4:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Telescope Design'!$N$4:$N$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D77E-41FB-92D3-5BB0E339E5EC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="474563616"/>
+        <c:axId val="474568208"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="474563616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="8"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>F/#</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="474568208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="474568208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>% Through</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="474563616"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EA631A0-CBF4-4135-91FC-24AEBB24A27A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1598,8 +2660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D396856-282B-40CF-8DBB-94DCDACCA298}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2952,10 +4014,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3767033-BADF-4D73-A126-394CBE3D01CB}">
-  <dimension ref="A2:M9"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2967,15 +4029,32 @@
     <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>236</v>
+      </c>
+      <c r="O1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>141</v>
       </c>
       <c r="B2" s="9"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>235</v>
+      </c>
+      <c r="O2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -3015,22 +4094,25 @@
       <c r="M3" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>'Spectrometer Design'!B13</f>
         <v>8000</v>
       </c>
       <c r="B4">
-        <f>D4/('Spectrometer Design'!B9/2)</f>
+        <f>D4/('Spectrometer Design'!B$9/2)</f>
         <v>0.26500000000000001</v>
       </c>
       <c r="C4">
-        <f>'Spectrometer Design'!B9/2/A4</f>
+        <f>'Spectrometer Design'!B$9/2/A4</f>
         <v>0.125</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D5" si="0">C4*E4</f>
+        <f t="shared" ref="D4" si="0">C4*E4</f>
         <v>265</v>
       </c>
       <c r="E4">
@@ -3042,89 +4124,258 @@
         <v>1470</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G5" si="3">1/H4</f>
+        <f t="shared" ref="G4" si="3">1/H4</f>
         <v>-2.5000000000000001E-4</v>
       </c>
       <c r="H4">
-        <f>'Spectrometer Design'!B14</f>
+        <f>'Spectrometer Design'!B$14</f>
         <v>-4000</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I5" si="4">(E4+F4-A4)/(2*F4*E4)</f>
+        <f t="shared" ref="I4" si="4">(E4+F4-A4)/(2*F4*E4)</f>
         <v>-7.0754716981132071E-4</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J5" si="5">1/I4</f>
+        <f t="shared" ref="J4" si="5">1/I4</f>
         <v>-1413.3333333333335</v>
       </c>
       <c r="K4">
-        <f>'Spectrometer Design'!B6</f>
+        <f>'Spectrometer Design'!B$6</f>
         <v>650</v>
       </c>
       <c r="L4">
-        <f>A4/'Spectrometer Design'!B9</f>
+        <f>A4/'Spectrometer Design'!B$9</f>
         <v>4</v>
       </c>
       <c r="M4" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>10000</v>
+      </c>
+      <c r="B5">
+        <f>D5/('Spectrometer Design'!B$9/2)</f>
+        <v>0.22083333333333333</v>
+      </c>
+      <c r="C5">
+        <f>'Spectrometer Design'!B$9/2/A5</f>
+        <v>0.1</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D4:D8" si="6">C5*E5</f>
+        <v>220.83333333333331</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E4:E5" si="7">F5+K5</f>
+        <v>2208.333333333333</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F4:F5" si="8">(K5-A5)/(2*A5*G5-1)</f>
+        <v>1558.3333333333333</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G4:G8" si="9">1/H5</f>
+        <v>-2.5000000000000001E-4</v>
+      </c>
+      <c r="H5">
+        <f>'Spectrometer Design'!B$14</f>
+        <v>-4000</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I4:I8" si="10">(E5+F5-A5)/(2*F5*E5)</f>
+        <v>-9.0566037735849078E-4</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J4:J8" si="11">1/I5</f>
+        <v>-1104.1666666666665</v>
+      </c>
+      <c r="K5">
+        <f>'Spectrometer Design'!B$6</f>
+        <v>650</v>
+      </c>
+      <c r="L5">
+        <f>A5/'Spectrometer Design'!B$9</f>
+        <v>5</v>
+      </c>
+      <c r="M5" t="s">
+        <v>150</v>
+      </c>
+      <c r="N5">
+        <v>57.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>12000</v>
+      </c>
+      <c r="B6">
+        <f>D6/('Spectrometer Design'!B$9/2)</f>
+        <v>0.18928571428571428</v>
+      </c>
+      <c r="C6">
+        <f>'Spectrometer Design'!B$9/2/A6</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D7" si="12">C6*E6</f>
+        <v>189.28571428571428</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E7" si="13">F6+K6</f>
+        <v>2271.4285714285716</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:F7" si="14">(K6-A6)/(2*A6*G6-1)</f>
+        <v>1621.4285714285713</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G7" si="15">1/H6</f>
+        <v>-2.5000000000000001E-4</v>
+      </c>
+      <c r="H6">
+        <f>'Spectrometer Design'!B$14</f>
+        <v>-4000</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I7" si="16">(E6+F6-A6)/(2*F6*E6)</f>
+        <v>-1.10062893081761E-3</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J7" si="17">1/I6</f>
+        <v>-908.57142857142856</v>
+      </c>
+      <c r="K6">
+        <f>'Spectrometer Design'!B$6</f>
+        <v>650</v>
+      </c>
+      <c r="L6">
+        <f>A6/'Spectrometer Design'!B$9</f>
+        <v>6</v>
+      </c>
+      <c r="M6" t="s">
+        <v>150</v>
+      </c>
+      <c r="N6">
+        <v>72.099999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>16000</v>
+      </c>
+      <c r="B7">
+        <f>D7/('Spectrometer Design'!B$9/2)</f>
+        <v>0.14722222222222223</v>
+      </c>
+      <c r="C7">
+        <f>'Spectrometer Design'!B$9/2/A7</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="12"/>
+        <v>147.22222222222223</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="13"/>
+        <v>2355.5555555555557</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="14"/>
+        <v>1705.5555555555557</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="15"/>
+        <v>-2.5000000000000001E-4</v>
+      </c>
+      <c r="H7">
+        <f>'Spectrometer Design'!B$14</f>
+        <v>-4000</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="16"/>
+        <v>-1.4858490566037733E-3</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="17"/>
+        <v>-673.01587301587313</v>
+      </c>
+      <c r="K7">
+        <f>'Spectrometer Design'!B$6</f>
+        <v>650</v>
+      </c>
+      <c r="L7">
+        <f>A7/'Spectrometer Design'!B$9</f>
+        <v>8</v>
+      </c>
+      <c r="M7" t="s">
+        <v>150</v>
+      </c>
+      <c r="N7">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>9698.82</v>
       </c>
-      <c r="B5">
-        <f>D5/('F Lambda Specs'!$B$9/2)</f>
+      <c r="B8">
+        <f>D8/('F Lambda Specs'!$B$9/2)</f>
         <v>0.23043636247728935</v>
       </c>
-      <c r="C5">
-        <f>'F Lambda Specs'!$B$9/2/A5</f>
+      <c r="C8">
+        <f>'F Lambda Specs'!$B$9/2/A8</f>
         <v>0.10310532621494162</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
+      <c r="D8">
+        <f t="shared" si="6"/>
         <v>230.43636247728935</v>
       </c>
-      <c r="E5">
-        <f>F5+K5</f>
+      <c r="E8">
+        <f>F8+K8</f>
         <v>2234.9608011219834</v>
       </c>
-      <c r="F5">
-        <f>(K5-A5)/(2*A5*G5-1)</f>
+      <c r="F8">
+        <f>(K8-A8)/(2*A8*G8-1)</f>
         <v>1589.9608011219836</v>
       </c>
-      <c r="G5">
-        <f t="shared" si="3"/>
+      <c r="G8">
+        <f t="shared" si="9"/>
         <v>-2.4200711016889679E-4</v>
       </c>
-      <c r="H5">
+      <c r="H8">
         <v>-4132.1099999999997</v>
       </c>
-      <c r="I5">
-        <f t="shared" si="4"/>
+      <c r="I8">
+        <f t="shared" si="10"/>
         <v>-8.2649476416811712E-4</v>
       </c>
-      <c r="J5">
-        <f t="shared" si="5"/>
+      <c r="J8">
+        <f t="shared" si="11"/>
         <v>-1209.9290199454792</v>
       </c>
-      <c r="K5">
+      <c r="K8">
         <v>645</v>
       </c>
-      <c r="L5">
-        <f>A5/'F Lambda Specs'!$B$9</f>
+      <c r="L8">
+        <f>A8/'F Lambda Specs'!$B$9</f>
         <v>4.8494099999999998</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update data in SW and use normalized efficiency within main beam
</commit_message>
<xml_diff>
--- a/optics_analysis/OpticalSpecifications.xlsx
+++ b/optics_analysis/OpticalSpecifications.xlsx
@@ -1,53 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\IODLab\Consulting\TIM\tim-inst_modl\optics_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C0016B-A50A-4AD2-A8F7-24D1F120ECC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C70480-5AB1-45C6-9F32-D2C427B429C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-8790" windowWidth="21840" windowHeight="38040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-8790" windowWidth="21840" windowHeight="38040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spectrometer Design" sheetId="1" r:id="rId1"/>
-    <sheet name="Telescope Design" sheetId="2" r:id="rId2"/>
-    <sheet name="F Lambda Specs" sheetId="3" r:id="rId3"/>
-    <sheet name="ResPow Specs" sheetId="4" r:id="rId4"/>
-    <sheet name="Ibsen Spectrometer Design" sheetId="5" r:id="rId5"/>
-    <sheet name="Old Calcs" sheetId="6" r:id="rId6"/>
+    <sheet name="Spectrometer As Built" sheetId="7" r:id="rId2"/>
+    <sheet name="Telescope Design" sheetId="2" r:id="rId3"/>
+    <sheet name="F Lambda Specs" sheetId="3" r:id="rId4"/>
+    <sheet name="ResPow Specs" sheetId="4" r:id="rId5"/>
+    <sheet name="Ibsen Spectrometer Design" sheetId="5" r:id="rId6"/>
+    <sheet name="Old Calcs" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="2">'F Lambda Specs'!$B$67</definedName>
-    <definedName name="solver_cvg" localSheetId="2">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="2">2</definedName>
-    <definedName name="solver_eng" localSheetId="2">1</definedName>
-    <definedName name="solver_est" localSheetId="2">1</definedName>
-    <definedName name="solver_itr" localSheetId="2">2147483647</definedName>
-    <definedName name="solver_mip" localSheetId="2">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="2">30</definedName>
-    <definedName name="solver_mrt" localSheetId="2">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="2">2</definedName>
-    <definedName name="solver_neg" localSheetId="2">1</definedName>
-    <definedName name="solver_nod" localSheetId="2">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="2">0</definedName>
-    <definedName name="solver_nwt" localSheetId="2">1</definedName>
-    <definedName name="solver_opt" localSheetId="2">'F Lambda Specs'!$B$69</definedName>
-    <definedName name="solver_pre" localSheetId="2">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="2">2</definedName>
-    <definedName name="solver_rlx" localSheetId="2">2</definedName>
-    <definedName name="solver_rsd" localSheetId="2">0</definedName>
-    <definedName name="solver_scl" localSheetId="2">2</definedName>
-    <definedName name="solver_sho" localSheetId="2">2</definedName>
-    <definedName name="solver_ssz" localSheetId="2">100</definedName>
-    <definedName name="solver_tim" localSheetId="2">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="2">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="2">3</definedName>
-    <definedName name="solver_val" localSheetId="2">0</definedName>
-    <definedName name="solver_ver" localSheetId="2">3</definedName>
+    <definedName name="solver_adj" localSheetId="3">'F Lambda Specs'!$B$67</definedName>
+    <definedName name="solver_cvg" localSheetId="3">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="3">2</definedName>
+    <definedName name="solver_eng" localSheetId="3">1</definedName>
+    <definedName name="solver_est" localSheetId="3">1</definedName>
+    <definedName name="solver_itr" localSheetId="3">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="3">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="3">30</definedName>
+    <definedName name="solver_mrt" localSheetId="3">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="3">2</definedName>
+    <definedName name="solver_neg" localSheetId="3">1</definedName>
+    <definedName name="solver_nod" localSheetId="3">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="3">0</definedName>
+    <definedName name="solver_nwt" localSheetId="3">1</definedName>
+    <definedName name="solver_opt" localSheetId="3">'F Lambda Specs'!$B$69</definedName>
+    <definedName name="solver_pre" localSheetId="3">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="3">2</definedName>
+    <definedName name="solver_rlx" localSheetId="3">2</definedName>
+    <definedName name="solver_rsd" localSheetId="3">0</definedName>
+    <definedName name="solver_scl" localSheetId="3">2</definedName>
+    <definedName name="solver_sho" localSheetId="3">2</definedName>
+    <definedName name="solver_ssz" localSheetId="3">100</definedName>
+    <definedName name="solver_tim" localSheetId="3">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="3">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="3">3</definedName>
+    <definedName name="solver_val" localSheetId="3">0</definedName>
+    <definedName name="solver_ver" localSheetId="3">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="243">
   <si>
     <t>TIM Balloon Optical Specifications</t>
   </si>
@@ -772,6 +773,30 @@
   </si>
   <si>
     <t>FFOV</t>
+  </si>
+  <si>
+    <t>Slit Width (F/# *Lambda)</t>
+  </si>
+  <si>
+    <t>Focal Plane</t>
+  </si>
+  <si>
+    <t>Grating</t>
+  </si>
+  <si>
+    <t>Slit</t>
+  </si>
+  <si>
+    <t>Min Wavelegnth</t>
+  </si>
+  <si>
+    <t>Spatial Pixel Pitch (F/#*Lambda)</t>
+  </si>
+  <si>
+    <t>Calculated at the smallest wavelength. At longer wavelengths, this means we resolve more than is necessary.</t>
+  </si>
+  <si>
+    <t>Calculated from the grating diameter and pitch (i.e. # of illuminated lines)</t>
   </si>
 </sst>
 </file>
@@ -785,7 +810,7 @@
     <numFmt numFmtId="167" formatCode="0.0000E+00"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -854,8 +879,28 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -872,6 +917,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -914,11 +964,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -980,12 +1031,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="2" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="37">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1133,6 +1198,76 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1664,10 +1799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2512,427 +2647,457 @@
         <v>84</v>
       </c>
       <c r="B73" s="13">
-        <f>1.5*B72*B46/1000</f>
-        <v>1.735604108928658</v>
+        <v>2</v>
       </c>
       <c r="C73" s="13">
-        <f>1.5*C72*C46/1000</f>
-        <v>1.9552358285436675</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B74" s="13">
+        <f>B73/($B$16*B10/1000)</f>
+        <v>2.0833333333333335</v>
+      </c>
+      <c r="C74" s="13">
+        <f>C73/($B$16*C10/1000)</f>
+        <v>2.3659305993690851</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B75" s="13">
+        <f>B74/($B$16*B11/1000)</f>
+        <v>1.6430073606729758</v>
+      </c>
+      <c r="C75" s="13">
+        <f>C74/($B$16*C11/1000)</f>
+        <v>1.4082920234339793</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B74" s="13">
+      <c r="B76" s="13">
         <f>B70*B45/1000</f>
         <v>1.019394655555814</v>
       </c>
-      <c r="C74" s="13">
+      <c r="C76" s="13">
         <f>C70*C45/1000</f>
         <v>1.1366248351102934</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="10" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="B75" s="13">
+      <c r="B77" s="13">
         <f>B71*B46/1000</f>
         <v>1.7236610170325892</v>
       </c>
-      <c r="C75" s="13">
+      <c r="C77" s="13">
         <f>C71*C46/1000</f>
         <v>1.9083975124368886</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D77" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="10" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B76" s="13">
-        <f>B$39/B74</f>
+      <c r="B78" s="13">
+        <f>B$39/B76</f>
         <v>2.2562409832784041</v>
       </c>
-      <c r="C76" s="13">
-        <f>C$39/C74</f>
+      <c r="C78" s="13">
+        <f>C$39/C76</f>
         <v>2.023534880598326</v>
       </c>
-      <c r="D76" s="1" t="s">
+      <c r="D78" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="10" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B77" s="13">
-        <f>B$39/B75</f>
+      <c r="B79" s="13">
+        <f>B$39/B77</f>
         <v>1.3343690999983402</v>
       </c>
-      <c r="C77" s="13">
-        <f>C$39/C75</f>
+      <c r="C79" s="13">
+        <f>C$39/C77</f>
         <v>1.2051996426379024</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="10" t="s">
+    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B78" s="13">
+      <c r="B80" s="13">
         <f>B72*B45/1000</f>
         <v>0.87601469220373906</v>
       </c>
-      <c r="C78" s="13">
+      <c r="C80" s="13">
         <f>C72*C45/1000</f>
         <v>0.98382501214022633</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="10" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B79" s="13">
+      <c r="B81" s="13">
         <f>B72*B46/1000</f>
         <v>1.1570694059524387</v>
       </c>
-      <c r="C79" s="13">
+      <c r="C81" s="13">
         <f>C72*C46/1000</f>
         <v>1.3034905523624449</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="10" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B80" s="13">
-        <f>B$41/B78</f>
+      <c r="B82" s="13">
+        <f>B$41/B80</f>
         <v>2.2737728561303081</v>
       </c>
-      <c r="C80" s="13">
-        <f>C$41/C78</f>
+      <c r="C82" s="13">
+        <f>C$41/C80</f>
         <v>2.0246064128529246</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="10" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B81" s="13">
-        <f>B$41/B79</f>
+      <c r="B83" s="13">
+        <f>B$41/B81</f>
         <v>1.7214684084267318</v>
       </c>
-      <c r="C81" s="13">
-        <f>C$41/C79</f>
+      <c r="C83" s="13">
+        <f>C$41/C81</f>
         <v>1.5280957925580407</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="10"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="11" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="10"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="11" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B84">
-        <v>240</v>
-      </c>
-      <c r="C84">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B85">
-        <f>B84+19.25</f>
-        <v>259.25</v>
-      </c>
-      <c r="C85">
-        <f>C84+25.75</f>
-        <v>342.75</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B86">
-        <f>B85+19.25</f>
-        <v>278.5</v>
+        <v>240</v>
       </c>
       <c r="C86">
-        <f>C85+25.75</f>
-        <v>368.5</v>
+        <v>317</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B87">
         <f>B86+19.25</f>
-        <v>297.75</v>
+        <v>259.25</v>
       </c>
       <c r="C87">
         <f>C86+25.75</f>
-        <v>394.25</v>
+        <v>342.75</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B88">
         <f>B87+19.25</f>
-        <v>317</v>
+        <v>278.5</v>
       </c>
       <c r="C88">
         <f>C87+25.75</f>
-        <v>420</v>
+        <v>368.5</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B89">
-        <v>3.2500000000000001E-2</v>
+        <f>B88+19.25</f>
+        <v>297.75</v>
       </c>
       <c r="C89">
-        <v>-3.2500000000000001E-2</v>
+        <f>C88+25.75</f>
+        <v>394.25</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B90">
-        <v>0</v>
+        <f>B89+19.25</f>
+        <v>317</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <f>C89+25.75</f>
+        <v>420</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B91" s="13">
-        <f>B92/2</f>
-        <v>0.23204790702798342</v>
-      </c>
-      <c r="C91" s="13">
-        <f>C92/2</f>
-        <v>0.2315752168470005</v>
+        <v>98</v>
+      </c>
+      <c r="B91">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="C91">
+        <v>-3.2500000000000001E-2</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B93" s="13">
+        <f>B94/2</f>
+        <v>0.23204790702798342</v>
+      </c>
+      <c r="C93" s="13">
+        <f>C94/2</f>
+        <v>0.2315752168470005</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B92" s="13">
+      <c r="B94" s="13">
         <f>B19</f>
         <v>0.46409581405596684</v>
       </c>
-      <c r="C92" s="13">
+      <c r="C94" s="13">
         <f>C19</f>
         <v>0.463150433694001</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="10" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B93" s="13">
-        <f>B94/2</f>
+      <c r="B95" s="13">
+        <f>B96/2</f>
         <v>-0.23204790702798342</v>
       </c>
-      <c r="C93" s="13">
-        <f>C94/2</f>
+      <c r="C95" s="13">
+        <f>C96/2</f>
         <v>-0.2315752168470005</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="10" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B94" s="13">
+      <c r="B96" s="13">
         <f>-B19</f>
         <v>-0.46409581405596684</v>
       </c>
-      <c r="C94" s="13">
+      <c r="C96" s="13">
         <f>-C19</f>
         <v>-0.463150433694001</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="B96">
-        <f>ASIN((B$50*B86*B$56+B$54*SIN(RADIANS(B$58)))/B$55)</f>
-        <v>0.69278552493770007</v>
-      </c>
-      <c r="C96">
-        <f>ASIN((C$50*C86*C$56+C$54*SIN(RADIANS(C$58)))/C$55)</f>
-        <v>0.67958533137844945</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="B97">
-        <f t="shared" ref="B97:C101" si="0">B$67 * TAN(ASIN((B$50*B84*B$56 + B$54*SIN(RADIANS(B$58)))/B$55) - B$96)</f>
-        <v>-64.759922002707356</v>
-      </c>
-      <c r="C97">
-        <f t="shared" si="0"/>
-        <v>-64.931254398486146</v>
-      </c>
-    </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B98">
-        <f t="shared" si="0"/>
-        <v>-33.020788336519892</v>
+        <f>ASIN((B$50*B88*B$56+B$54*SIN(RADIANS(B$58)))/B$55)</f>
+        <v>0.69278552493770007</v>
       </c>
       <c r="C98">
-        <f t="shared" si="0"/>
-        <v>-33.082447813430207</v>
+        <f>ASIN((C$50*C88*C$56+C$54*SIN(RADIANS(C$58)))/C$55)</f>
+        <v>0.67958533137844945</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B99">
-        <f>B$67 * TAN(ASIN((B$50*B86*B$56 + B$54*SIN(RADIANS(B$58)))/B$55) - B$96)</f>
-        <v>0</v>
+        <f>B$67 * TAN(ASIN((B$50*B86*B$56 + B$54*SIN(RADIANS(B$58)))/B$55) - B$98)</f>
+        <v>-64.759922002707356</v>
       </c>
       <c r="C99">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C$67 * TAN(ASIN((C$50*C86*C$56 + C$54*SIN(RADIANS(C$58)))/C$55) - C$98)</f>
+        <v>-64.931254398486146</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B100">
-        <f t="shared" si="0"/>
-        <v>35.057157711666186</v>
+        <f>B$67 * TAN(ASIN((B$50*B87*B$56 + B$54*SIN(RADIANS(B$58)))/B$55) - B$98)</f>
+        <v>-33.020788336519892</v>
       </c>
       <c r="C100">
-        <f t="shared" si="0"/>
-        <v>35.03998287561857</v>
+        <f>C$67 * TAN(ASIN((C$50*C87*C$56 + C$54*SIN(RADIANS(C$58)))/C$55) - C$98)</f>
+        <v>-33.082447813430207</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B101">
-        <f t="shared" si="0"/>
-        <v>73.250896295617295</v>
+        <f>B$67 * TAN(ASIN((B$50*B88*B$56 + B$54*SIN(RADIANS(B$58)))/B$55) - B$98)</f>
+        <v>0</v>
       </c>
       <c r="C101">
-        <f t="shared" si="0"/>
-        <v>73.078441963971798</v>
+        <f>C$67 * TAN(ASIN((C$50*C88*C$56 + C$54*SIN(RADIANS(C$58)))/C$55) - C$98)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B102">
+        <f>B$67 * TAN(ASIN((B$50*B89*B$56 + B$54*SIN(RADIANS(B$58)))/B$55) - B$98)</f>
+        <v>35.057157711666186</v>
+      </c>
+      <c r="C102">
+        <f>C$67 * TAN(ASIN((C$50*C89*C$56 + C$54*SIN(RADIANS(C$58)))/C$55) - C$98)</f>
+        <v>35.03998287561857</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="B103" s="15">
-        <f>B$67 * TAN(B90*$B$13/B$62)</f>
-        <v>0</v>
-      </c>
-      <c r="C103" s="15">
-        <f>C$67 * TAN(C90*$B$13/C$62)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="B104" s="15">
-        <f t="shared" ref="B104:C107" si="1">B$67 * TAN(RADIANS(B91*$B$13/B$62))</f>
-        <v>29.838455496169814</v>
-      </c>
-      <c r="C104" s="15">
-        <f t="shared" si="1"/>
-        <v>25.309175077201669</v>
+        <v>109</v>
+      </c>
+      <c r="B103">
+        <f>B$67 * TAN(ASIN((B$50*B90*B$56 + B$54*SIN(RADIANS(B$58)))/B$55) - B$98)</f>
+        <v>73.250896295617295</v>
+      </c>
+      <c r="C103">
+        <f>C$67 * TAN(ASIN((C$50*C90*C$56 + C$54*SIN(RADIANS(C$58)))/C$55) - C$98)</f>
+        <v>73.078441963971798</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B105" s="15">
-        <f t="shared" si="1"/>
-        <v>59.913826086925553</v>
+        <f>B$67 * TAN(B92*$B$13/B$62)</f>
+        <v>0</v>
       </c>
       <c r="C105" s="15">
-        <f t="shared" si="1"/>
-        <v>50.758853671139683</v>
+        <f>C$67 * TAN(C92*$B$13/C$62)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B106" s="15">
-        <f t="shared" si="1"/>
-        <v>-29.838455496169814</v>
+        <f t="shared" ref="B106:C109" si="0">B$67 * TAN(RADIANS(B93*$B$13/B$62))</f>
+        <v>29.838455496169814</v>
       </c>
       <c r="C106" s="15">
-        <f t="shared" si="1"/>
-        <v>-25.309175077201669</v>
+        <f t="shared" si="0"/>
+        <v>25.309175077201669</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B107" s="15">
+        <f t="shared" si="0"/>
+        <v>59.913826086925553</v>
+      </c>
+      <c r="C107" s="15">
+        <f t="shared" si="0"/>
+        <v>50.758853671139683</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B108" s="15">
+        <f t="shared" si="0"/>
+        <v>-29.838455496169814</v>
+      </c>
+      <c r="C108" s="15">
+        <f t="shared" si="0"/>
+        <v>-25.309175077201669</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="B107" s="15">
-        <f t="shared" si="1"/>
+      <c r="B109" s="15">
+        <f t="shared" si="0"/>
         <v>-59.913826086925553</v>
       </c>
-      <c r="C107" s="15">
-        <f>C$67 * TAN(RADIANS(C94*$B$13/C$62))</f>
+      <c r="C109" s="15">
+        <f>C$67 * TAN(RADIANS(C96*$B$13/C$62))</f>
         <v>-50.758853671139683</v>
       </c>
     </row>
@@ -2941,33 +3106,33 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <conditionalFormatting sqref="B66:C66">
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="notBetween">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="notBetween">
       <formula>$B$38-0.01*$B$38</formula>
       <formula>$B$38+0.01*$B$38</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="between">
       <formula>$B$38-0.01*$B$38</formula>
       <formula>$B$38+0.01*$B$38</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="greaterThan">
       <formula>$B$4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69">
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="greaterThan">
       <formula>$B$42</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="lessThan">
       <formula>$B$42</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69">
-    <cfRule type="cellIs" dxfId="24" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="7" operator="lessThan">
       <formula>$C$42</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="8" operator="greaterThan">
       <formula>$C$42</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2977,6 +3142,1603 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3824768D-5964-45D6-ABF4-96D18DC36DE7}">
+  <dimension ref="A1:G124"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="77.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="15"/>
+    <col min="7" max="7" width="14.140625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="14" style="15" customWidth="1"/>
+    <col min="9" max="1025" width="8.5703125" style="15" customWidth="1"/>
+    <col min="1026" max="16384" width="9.140625" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="7">
+        <v>2000</v>
+      </c>
+      <c r="C4" s="7">
+        <v>2000</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="15">
+        <v>510</v>
+      </c>
+      <c r="C5" s="15">
+        <v>510</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="7">
+        <v>650</v>
+      </c>
+      <c r="C6" s="7">
+        <v>650</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="15">
+        <v>2000</v>
+      </c>
+      <c r="C9" s="15">
+        <v>2000</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="15">
+        <v>240</v>
+      </c>
+      <c r="C10" s="15">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="15">
+        <v>317</v>
+      </c>
+      <c r="C11" s="15">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="15">
+        <f>B10/(1000*B9)</f>
+        <v>1.2E-4</v>
+      </c>
+      <c r="C12" s="15">
+        <f>C10/(1000*C9)</f>
+        <v>1.585E-4</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="15">
+        <v>8000</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="15">
+        <v>-3200</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="15">
+        <f>'Telescope Design'!J4</f>
+        <v>-937.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="15">
+        <f>B13/B9</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="15">
+        <f>ASIN(1/(2*B16))</f>
+        <v>0.12532783116806537</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="15">
+        <v>2.25</v>
+      </c>
+      <c r="C18" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="15">
+        <f>DEGREES(B36/2*B12)*B18</f>
+        <v>0.49503553499303132</v>
+      </c>
+      <c r="C19" s="15">
+        <f>DEGREES(C36/2*C12)*C18</f>
+        <v>0.463150433694001</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="15">
+        <f>2*B13*TAN(RADIANS(B19))</f>
+        <v>138.24343995628459</v>
+      </c>
+      <c r="C20" s="15">
+        <f>2*B13*TAN(RADIANS(C19))</f>
+        <v>129.33881713985178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="15">
+        <f>B20/2</f>
+        <v>69.121719978142295</v>
+      </c>
+      <c r="C21" s="15">
+        <f>C20/2</f>
+        <v>64.669408569925892</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="15">
+        <f>100*(B5/B9)^2</f>
+        <v>6.5024999999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="15">
+        <v>1</v>
+      </c>
+      <c r="C26" s="15">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="15">
+        <f>B26*B20</f>
+        <v>138.24343995628459</v>
+      </c>
+      <c r="C27" s="15">
+        <f>C26*C20</f>
+        <v>129.33881713985178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="15">
+        <f>B27/2</f>
+        <v>69.121719978142295</v>
+      </c>
+      <c r="C28" s="15">
+        <f>C27/2</f>
+        <v>64.669408569925892</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="15">
+        <f>5/60*SQRT(2)</f>
+        <v>0.11785113019775792</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="15">
+        <v>64</v>
+      </c>
+      <c r="C36" s="15">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="15">
+        <v>63</v>
+      </c>
+      <c r="C37" s="15">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="17">
+        <f>B42/B43</f>
+        <v>0.87977183876514409</v>
+      </c>
+      <c r="C38" s="17">
+        <f>C42/C43</f>
+        <v>0.70106818401597426</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="15">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C39" s="15">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="17">
+        <f>SQRT(3)/2</f>
+        <v>0.8660254037844386</v>
+      </c>
+      <c r="C40" s="17">
+        <f>SQRT(3)/2</f>
+        <v>0.8660254037844386</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="17">
+        <f>B39*B40</f>
+        <v>1.9918584287042087</v>
+      </c>
+      <c r="C41" s="17">
+        <f>C39*C40</f>
+        <v>1.9918584287042087</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="17">
+        <f>B39*B36*B40</f>
+        <v>127.47893943706936</v>
+      </c>
+      <c r="C42" s="17">
+        <f>C39*C36*C40</f>
+        <v>101.58477986391465</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="15">
+        <f>B39*B37</f>
+        <v>144.89999999999998</v>
+      </c>
+      <c r="C43" s="15">
+        <f>C39*C37</f>
+        <v>144.89999999999998</v>
+      </c>
+      <c r="E43" s="8"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="15">
+        <v>3.7</v>
+      </c>
+      <c r="C44" s="15">
+        <v>3.15</v>
+      </c>
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="B45" s="15">
+        <v>4.3</v>
+      </c>
+      <c r="C45" s="15">
+        <v>3.68</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E45" s="8"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="B46" s="15">
+        <v>5.4</v>
+      </c>
+      <c r="C46" s="15">
+        <v>4.5</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="B47" s="17">
+        <f>B$41/(B$44*B10/1000)</f>
+        <v>2.2430838161083431</v>
+      </c>
+      <c r="C47" s="17">
+        <f>C$41/(C$44*C10/1000)</f>
+        <v>1.9947508173894235</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="B48" s="17">
+        <f>B$41/(B$44*B11/1000)</f>
+        <v>1.6982338039936982</v>
+      </c>
+      <c r="C48" s="17">
+        <f>C$41/(C$44*C11/1000)</f>
+        <v>1.5055619264582076</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" s="8"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B49" s="17">
+        <f>B$39/(B45*B10/1000)</f>
+        <v>2.2286821705426356</v>
+      </c>
+      <c r="C49" s="17">
+        <f>C$39/(C45*C10/1000)</f>
+        <v>1.9716088328075707</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E49" s="8"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="17">
+        <f>B$39/(B46*B11/1000)</f>
+        <v>1.3436149082836777</v>
+      </c>
+      <c r="C50" s="17">
+        <f>C$39/(C46*C11/1000)</f>
+        <v>1.216931216931217</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E50" s="8"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" s="8"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" s="15">
+        <f>B10</f>
+        <v>240</v>
+      </c>
+      <c r="C52" s="15">
+        <f>C10</f>
+        <v>317</v>
+      </c>
+      <c r="E52" s="8"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" s="15">
+        <f>B11</f>
+        <v>317</v>
+      </c>
+      <c r="C53" s="15">
+        <f>C11</f>
+        <v>420</v>
+      </c>
+      <c r="E53" s="8"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" s="15">
+        <f>AVERAGE(B52:B53)</f>
+        <v>278.5</v>
+      </c>
+      <c r="C54" s="15">
+        <f>AVERAGE(C52:C53)</f>
+        <v>368.5</v>
+      </c>
+      <c r="E54" s="8"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" s="15">
+        <f>B53-B52</f>
+        <v>77</v>
+      </c>
+      <c r="C55" s="15">
+        <f>C53-C52</f>
+        <v>103</v>
+      </c>
+      <c r="E55" s="8"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E56" s="8"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B57" s="15">
+        <v>-1</v>
+      </c>
+      <c r="C57" s="15">
+        <v>-1</v>
+      </c>
+      <c r="E57" s="8"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="15">
+        <v>2.8549999999999999E-3</v>
+      </c>
+      <c r="C58" s="15">
+        <v>2.1299999999999999E-3</v>
+      </c>
+      <c r="E58" s="8"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="B59" s="23">
+        <v>150</v>
+      </c>
+      <c r="C59" s="23">
+        <v>190</v>
+      </c>
+      <c r="E59" s="8"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60" s="35">
+        <v>9</v>
+      </c>
+      <c r="C60" s="23">
+        <v>9</v>
+      </c>
+      <c r="E60" s="8"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" s="17">
+        <f>ABS(B57)*B59*1000*B58</f>
+        <v>428.25</v>
+      </c>
+      <c r="C61" s="17">
+        <f>ABS(C57)*C74*1000*C71</f>
+        <v>334.26536127890915</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62" s="17">
+        <f>B52/B61</f>
+        <v>0.56042031523642732</v>
+      </c>
+      <c r="C62" s="17">
+        <f>C52/C61</f>
+        <v>0.94834833853902367</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64" s="17">
+        <v>2</v>
+      </c>
+      <c r="C64" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="B65" s="17">
+        <f>B64/($B$16*B10/1000)</f>
+        <v>2.0833333333333335</v>
+      </c>
+      <c r="C65" s="17">
+        <f>C64/($B$16*C10/1000)</f>
+        <v>2.3659305993690851</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="B66" s="17">
+        <f>B65/($B$16*B11/1000)</f>
+        <v>1.6430073606729758</v>
+      </c>
+      <c r="C66" s="17">
+        <f>C65/($B$16*C11/1000)</f>
+        <v>1.4082920234339793</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="32"/>
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B68" s="17"/>
+      <c r="C68" s="17"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B69" s="15">
+        <v>1</v>
+      </c>
+      <c r="C69" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B70" s="15">
+        <v>-1</v>
+      </c>
+      <c r="C70" s="15">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B71" s="15">
+        <v>2.8549999999999999E-3</v>
+      </c>
+      <c r="C71" s="15">
+        <v>2.1299999999999999E-3</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72" s="15">
+        <v>130</v>
+      </c>
+      <c r="C72" s="15">
+        <v>155</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B73" s="15">
+        <v>9</v>
+      </c>
+      <c r="C73" s="15">
+        <v>9</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B74" s="13">
+        <f>B72/COS(RADIANS(B73))</f>
+        <v>131.62046635244039</v>
+      </c>
+      <c r="C74" s="13">
+        <f>C72/COS(RADIANS(C73))</f>
+        <v>156.93209449714044</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" s="13">
+        <f>DEGREES(ASIN((B$57*B$52*B$71 + B$69*SIN(RADIANS(B$73)))/B$70))</f>
+        <v>31.922084885300261</v>
+      </c>
+      <c r="C75" s="13">
+        <f>DEGREES(ASIN((C57*C52*C71 + C69*SIN(RADIANS(C73)))/C70))</f>
+        <v>31.250152590106154</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B76" s="13">
+        <f>DEGREES(ASIN((B$57*B$53*B$71 + B$69*SIN(RADIANS(B$73)))/B$70))</f>
+        <v>48.469296901370093</v>
+      </c>
+      <c r="C76" s="13">
+        <f>DEGREES(ASIN((C$57*C$53*C$71 + C$69*SIN(RADIANS(C$73)))/C$70))</f>
+        <v>47.575380872881681</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77" s="13">
+        <f>B72/(2*TAN(ASIN(1/(2*$B16))))</f>
+        <v>515.92150565759528</v>
+      </c>
+      <c r="C77" s="13">
+        <f>C72/(2*TAN(ASIN(1/(2*$B16))))</f>
+        <v>615.1371798225174</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B78" s="13">
+        <f>2*B77</f>
+        <v>1031.8430113151906</v>
+      </c>
+      <c r="C78" s="13">
+        <f>2*C77</f>
+        <v>1230.2743596450348</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B79" s="13">
+        <f>DEGREES(ASIN((B57*B53*B71+B69*SIN(RADIANS(B73)))/B70) - ASIN((B57*B52*B71+B69*SIN(RADIANS(B73)))/B70))</f>
+        <v>16.547212016069835</v>
+      </c>
+      <c r="C79" s="13">
+        <f>DEGREES(ASIN((C57*C53*C71+C69*SIN(RADIANS(C73)))/C70) - ASIN((C57*C52*C71+C69*SIN(RADIANS(C73)))/C70))</f>
+        <v>16.32522828277553</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B80" s="13">
+        <f>2*DEGREES(ATAN($B$28/B77))</f>
+        <v>15.261773803834579</v>
+      </c>
+      <c r="C80" s="13">
+        <f>2*DEGREES(ATAN($C$28/C77))</f>
+        <v>12.002926945070323</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B81" s="13">
+        <f>B80/B79</f>
+        <v>0.92231693103424905</v>
+      </c>
+      <c r="C81" s="13">
+        <f>C80/C79</f>
+        <v>0.73523792360897067</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B82" s="13">
+        <f>B43/(2*TAN(RADIANS(B79/2)))</f>
+        <v>498.23335619087646</v>
+      </c>
+      <c r="C82" s="13">
+        <f>C43/(2*TAN(RADIANS(C79/2)))</f>
+        <v>505.10258904044736</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B83" s="13">
+        <f>2*B82</f>
+        <v>996.46671238175293</v>
+      </c>
+      <c r="C83" s="13">
+        <f>2*C82</f>
+        <v>1010.2051780808947</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A84" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B84" s="13">
+        <f>2*B82*TAN(RADIANS(B80/2))</f>
+        <v>133.50382239445534</v>
+      </c>
+      <c r="C84" s="13">
+        <f>2*C82*TAN(RADIANS(C80/2))</f>
+        <v>106.20293089684043</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B85" s="13">
+        <f>B$82/(B$74*COS(RADIANS(B75)))</f>
+        <v>4.4598516180566863</v>
+      </c>
+      <c r="C85" s="13">
+        <f>C$82/(C$74*COS(RADIANS(C75)))</f>
+        <v>3.7648456683463967</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B86" s="13">
+        <f>B$82/(B$74*COS(RADIANS(B76)))</f>
+        <v>5.7092872803918562</v>
+      </c>
+      <c r="C86" s="13">
+        <f>C$82/(C$74*COS(RADIANS(C76)))</f>
+        <v>4.7709937810922209</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B87" s="13">
+        <f>B82/B72</f>
+        <v>3.8325642783913576</v>
+      </c>
+      <c r="C87" s="13">
+        <f>C82/C72</f>
+        <v>3.2587263809061118</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B88" s="13">
+        <v>2</v>
+      </c>
+      <c r="C88" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B89" s="13">
+        <f>B88/($B$16*B10/1000)</f>
+        <v>2.0833333333333335</v>
+      </c>
+      <c r="C89" s="13">
+        <f>C88/($B$16*C10/1000)</f>
+        <v>2.3659305993690851</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B90" s="13">
+        <f>B89/($B$16*B11/1000)</f>
+        <v>1.6430073606729758</v>
+      </c>
+      <c r="C90" s="13">
+        <f>C89/($B$16*C11/1000)</f>
+        <v>1.4082920234339793</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B91" s="13">
+        <f>B85*B52/1000</f>
+        <v>1.0703643883336047</v>
+      </c>
+      <c r="C91" s="13">
+        <f>C85*C52/1000</f>
+        <v>1.1934560768658078</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B92" s="13">
+        <f>B86*B53/1000</f>
+        <v>1.8098440678842185</v>
+      </c>
+      <c r="C92" s="13">
+        <f>C86*C53/1000</f>
+        <v>2.0038173880587329</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B93" s="13">
+        <f>B$39/B91</f>
+        <v>2.1488009364556229</v>
+      </c>
+      <c r="C93" s="13">
+        <f>C$39/C91</f>
+        <v>1.9271760767603112</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B94" s="13">
+        <f>B$39/B92</f>
+        <v>1.2708277142841338</v>
+      </c>
+      <c r="C94" s="13">
+        <f>C$39/C92</f>
+        <v>1.1478091834646689</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B95" s="13">
+        <f>B87*B52/1000</f>
+        <v>0.91981542681392581</v>
+      </c>
+      <c r="C95" s="13">
+        <f>C87*C52/1000</f>
+        <v>1.0330162627472375</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B96" s="13">
+        <f>B87*B53/1000</f>
+        <v>1.2149228762500603</v>
+      </c>
+      <c r="C96" s="13">
+        <f>C87*C53/1000</f>
+        <v>1.3686650799805671</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B97" s="13">
+        <f>B$41/B95</f>
+        <v>2.1654979582193419</v>
+      </c>
+      <c r="C97" s="13">
+        <f>C$41/C95</f>
+        <v>1.9281965836694523</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B98" s="13">
+        <f>B$41/B96</f>
+        <v>1.6394937223111736</v>
+      </c>
+      <c r="C98" s="13">
+        <f>C$41/C96</f>
+        <v>1.4553293262457532</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="10"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B101" s="15">
+        <v>240</v>
+      </c>
+      <c r="C101" s="15">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B102" s="15">
+        <f>B101+19.25</f>
+        <v>259.25</v>
+      </c>
+      <c r="C102" s="15">
+        <f>C101+25.75</f>
+        <v>342.75</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B103" s="15">
+        <f>B102+19.25</f>
+        <v>278.5</v>
+      </c>
+      <c r="C103" s="15">
+        <f>C102+25.75</f>
+        <v>368.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B104" s="15">
+        <f>B103+19.25</f>
+        <v>297.75</v>
+      </c>
+      <c r="C104" s="15">
+        <f>C103+25.75</f>
+        <v>394.25</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B105" s="15">
+        <f>B104+19.25</f>
+        <v>317</v>
+      </c>
+      <c r="C105" s="15">
+        <f>C104+25.75</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B106" s="15">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="C106" s="15">
+        <v>-3.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B107" s="15">
+        <v>0</v>
+      </c>
+      <c r="C107" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B108" s="13">
+        <f>B109/2</f>
+        <v>0.24751776749651566</v>
+      </c>
+      <c r="C108" s="13">
+        <f>C109/2</f>
+        <v>0.2315752168470005</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B109" s="13">
+        <f>B19</f>
+        <v>0.49503553499303132</v>
+      </c>
+      <c r="C109" s="13">
+        <f>C19</f>
+        <v>0.463150433694001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B110" s="13">
+        <f>B111/2</f>
+        <v>-0.24751776749651566</v>
+      </c>
+      <c r="C110" s="13">
+        <f>C111/2</f>
+        <v>-0.2315752168470005</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B111" s="13">
+        <f>-B19</f>
+        <v>-0.49503553499303132</v>
+      </c>
+      <c r="C111" s="13">
+        <f>-C19</f>
+        <v>-0.463150433694001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B113" s="15">
+        <f>ASIN((B$57*B103*B$71+B$69*SIN(RADIANS(B$73)))/B$70)</f>
+        <v>0.69278552493770007</v>
+      </c>
+      <c r="C113" s="15">
+        <f>ASIN((C$57*C103*C$71+C$69*SIN(RADIANS(C$73)))/C$70)</f>
+        <v>0.67958533137844945</v>
+      </c>
+      <c r="E113" s="15"/>
+      <c r="F113" s="15"/>
+      <c r="G113" s="15"/>
+    </row>
+    <row r="114" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B114" s="15">
+        <f>B$82 * TAN(ASIN((B$57*B101*B$71 + B$69*SIN(RADIANS(B$73)))/B$70) - B$113)</f>
+        <v>-67.997918102842718</v>
+      </c>
+      <c r="C114" s="15">
+        <f>C$82 * TAN(ASIN((C$57*C101*C$71 + C$69*SIN(RADIANS(C$73)))/C$70) - C$113)</f>
+        <v>-68.177817118410445</v>
+      </c>
+      <c r="E114" s="15"/>
+      <c r="F114" s="15"/>
+      <c r="G114" s="15"/>
+    </row>
+    <row r="115" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B115" s="15">
+        <f>B$82 * TAN(ASIN((B$57*B102*B$71 + B$69*SIN(RADIANS(B$73)))/B$70) - B$113)</f>
+        <v>-34.67182775334588</v>
+      </c>
+      <c r="C115" s="15">
+        <f>C$82 * TAN(ASIN((C$57*C102*C$71 + C$69*SIN(RADIANS(C$73)))/C$70) - C$113)</f>
+        <v>-34.736570204101717</v>
+      </c>
+      <c r="E115" s="15"/>
+      <c r="F115" s="15"/>
+      <c r="G115" s="15"/>
+    </row>
+    <row r="116" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B116" s="15">
+        <f>B$82 * TAN(ASIN((B$57*B103*B$71 + B$69*SIN(RADIANS(B$73)))/B$70) - B$113)</f>
+        <v>0</v>
+      </c>
+      <c r="C116" s="15">
+        <f>C$82 * TAN(ASIN((C$57*C103*C$71 + C$69*SIN(RADIANS(C$73)))/C$70) - C$113)</f>
+        <v>0</v>
+      </c>
+      <c r="E116" s="15"/>
+      <c r="F116" s="15"/>
+      <c r="G116" s="15"/>
+    </row>
+    <row r="117" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B117" s="15">
+        <f>B$82 * TAN(ASIN((B$57*B104*B$71 + B$69*SIN(RADIANS(B$73)))/B$70) - B$113)</f>
+        <v>36.810015597249489</v>
+      </c>
+      <c r="C117" s="15">
+        <f>C$82 * TAN(ASIN((C$57*C104*C$71 + C$69*SIN(RADIANS(C$73)))/C$70) - C$113)</f>
+        <v>36.791982019399491</v>
+      </c>
+      <c r="E117" s="15"/>
+      <c r="F117" s="15"/>
+      <c r="G117" s="15"/>
+    </row>
+    <row r="118" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B118" s="15">
+        <f>B$82 * TAN(ASIN((B$57*B105*B$71 + B$69*SIN(RADIANS(B$73)))/B$70) - B$113)</f>
+        <v>76.913441110398153</v>
+      </c>
+      <c r="C118" s="15">
+        <f>C$82 * TAN(ASIN((C$57*C105*C$71 + C$69*SIN(RADIANS(C$73)))/C$70) - C$113)</f>
+        <v>76.732364062170376</v>
+      </c>
+      <c r="E118" s="15"/>
+      <c r="F118" s="15"/>
+      <c r="G118" s="15"/>
+    </row>
+    <row r="120" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B120" s="15">
+        <f>B$82 * TAN(B107*$B$13/B$77)</f>
+        <v>0</v>
+      </c>
+      <c r="C120" s="15">
+        <f>C$82 * TAN(C107*$B$13/C$77)</f>
+        <v>0</v>
+      </c>
+      <c r="E120" s="15"/>
+      <c r="F120" s="15"/>
+      <c r="G120" s="15"/>
+    </row>
+    <row r="121" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B121" s="15">
+        <f>B$82 * TAN(RADIANS(B108*$B$13/B$77))</f>
+        <v>33.425135696144217</v>
+      </c>
+      <c r="C121" s="15">
+        <f>C$82 * TAN(RADIANS(C108*$B$13/C$77))</f>
+        <v>26.57463383106175</v>
+      </c>
+      <c r="E121" s="15"/>
+      <c r="F121" s="15"/>
+      <c r="G121" s="15"/>
+    </row>
+    <row r="122" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B122" s="15">
+        <f>B$82 * TAN(RADIANS(B109*$B$13/B$77))</f>
+        <v>67.152505154646747</v>
+      </c>
+      <c r="C122" s="15">
+        <f>C$82 * TAN(RADIANS(C109*$B$13/C$77))</f>
+        <v>53.296796354696653</v>
+      </c>
+      <c r="E122" s="15"/>
+      <c r="F122" s="15"/>
+      <c r="G122" s="15"/>
+    </row>
+    <row r="123" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B123" s="15">
+        <f>B$82 * TAN(RADIANS(B110*$B$13/B$77))</f>
+        <v>-33.425135696144217</v>
+      </c>
+      <c r="C123" s="15">
+        <f>C$82 * TAN(RADIANS(C110*$B$13/C$77))</f>
+        <v>-26.57463383106175</v>
+      </c>
+      <c r="E123" s="15"/>
+      <c r="F123" s="15"/>
+      <c r="G123" s="15"/>
+    </row>
+    <row r="124" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B124" s="15">
+        <f>B$82 * TAN(RADIANS(B111*$B$13/B$77))</f>
+        <v>-67.152505154646747</v>
+      </c>
+      <c r="C124" s="15">
+        <f>C$82 * TAN(RADIANS(C111*$B$13/C$77))</f>
+        <v>-53.296796354696653</v>
+      </c>
+      <c r="E124" s="15"/>
+      <c r="F124" s="15"/>
+      <c r="G124" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B81:C81">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="notBetween">
+      <formula>$B$38-0.01*$B$38</formula>
+      <formula>$B$38+0.01*$B$38</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="between">
+      <formula>$B$38-0.01*$B$38</formula>
+      <formula>$B$38+0.01*$B$38</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="greaterThan">
+      <formula>$B$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B84">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="greaterThan">
+      <formula>$B$42</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="lessThan">
+      <formula>$B$42</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C84">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="lessThan">
+      <formula>$C$42</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="7" operator="greaterThan">
+      <formula>$C$42</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:M8"/>
   <sheetViews>
@@ -3311,7 +5073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G85"/>
   <sheetViews>
@@ -4407,7 +6169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G75"/>
   <sheetViews>
@@ -5372,7 +7134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
@@ -6115,7 +7877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H58"/>
   <sheetViews>

</xml_diff>

<commit_message>
Include out of band POP analysis data
</commit_message>
<xml_diff>
--- a/optics_analysis/OpticalSpecifications.xlsx
+++ b/optics_analysis/OpticalSpecifications.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\IODLab\Consulting\TIM\tim-inst_modl\optics_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C70480-5AB1-45C6-9F32-D2C427B429C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEAF1D8-E2C5-416D-988F-7F13160E6700}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-8790" windowWidth="21840" windowHeight="38040" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="623" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spectrometer Design" sheetId="1" r:id="rId1"/>
@@ -1025,12 +1025,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1044,6 +1038,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1805,27 +1805,27 @@
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="77.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="34.73046875" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" customWidth="1"/>
+    <col min="3" max="3" width="20.73046875" customWidth="1"/>
+    <col min="4" max="4" width="77.86328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" customWidth="1"/>
+    <col min="6" max="6" width="11.3984375"/>
+    <col min="7" max="7" width="14.1328125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="9" max="1025" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.65">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1839,14 +1839,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -1888,19 +1888,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>-937.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>0.12532783116806537</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>129.33881713985178</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>64.669408569925892</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -2063,12 +2063,12 @@
         <v>6.5024999999999995</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>35</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>129.33881713985178</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -2116,12 +2116,12 @@
         <v>64.669408569925892</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>0.11785113019775792</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>40</v>
       </c>
@@ -2151,12 +2151,12 @@
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>41</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>42</v>
       </c>
@@ -2178,7 +2178,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="10" t="s">
         <v>43</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>0.73612159321677284</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>44</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>45</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>0.8660254037844386</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -2228,7 +2228,7 @@
         <v>1.9918584287042087</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="10" t="s">
         <v>47</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>101.58477986391465</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="10" t="s">
         <v>48</v>
       </c>
@@ -2255,13 +2255,13 @@
       </c>
       <c r="E43" s="8"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E44" s="8"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -2275,7 +2275,7 @@
       </c>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -2289,7 +2289,7 @@
       </c>
       <c r="E46" s="8"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="10" t="s">
         <v>49</v>
       </c>
@@ -2303,7 +2303,7 @@
       </c>
       <c r="E47" s="8"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="10" t="s">
         <v>50</v>
       </c>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="E48" s="8"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="10" t="s">
         <v>33</v>
       </c>
@@ -2329,7 +2329,7 @@
       </c>
       <c r="E49" s="8"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="9" t="s">
         <v>52</v>
       </c>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="E50" s="8"/>
     </row>
-    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A52" s="10" t="s">
         <v>55</v>
       </c>
@@ -2373,12 +2373,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" s="9" t="s">
         <v>58</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
         <v>59</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="9" t="s">
         <v>60</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A57" s="9" t="s">
         <v>62</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" s="9" t="s">
         <v>64</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>156.93209449714044</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60" s="10" t="s">
         <v>66</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" s="10" t="s">
         <v>66</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" s="10" t="s">
         <v>69</v>
       </c>
@@ -2500,7 +2500,7 @@
         <v>615.1371798225174</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" s="10" t="s">
         <v>70</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>1230.2743596450348</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" s="10" t="s">
         <v>71</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="10" t="s">
         <v>73</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>12.002926945070323</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A66" s="10" t="s">
         <v>74</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="10" t="s">
         <v>76</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="10" t="s">
         <v>78</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>962.10016960085227</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A69" s="14" t="s">
         <v>79</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" s="10" t="s">
         <v>81</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>3.585567303187045</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="10" t="s">
         <v>82</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>4.543803601040211</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" s="10" t="s">
         <v>83</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>3.1035489341962976</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" s="10" t="s">
         <v>84</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A74" s="10" t="s">
         <v>235</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A75" s="10" t="s">
         <v>235</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" s="10" t="s">
         <v>85</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" s="10" t="s">
         <v>85</v>
       </c>
@@ -2717,7 +2717,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" s="10" t="s">
         <v>88</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" s="10" t="s">
         <v>88</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A80" s="10" t="s">
         <v>89</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" s="10" t="s">
         <v>89</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" s="10" t="s">
         <v>91</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" s="10" t="s">
         <v>91</v>
       </c>
@@ -2813,15 +2813,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" s="10"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" s="11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" s="10" t="s">
         <v>93</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" s="10" t="s">
         <v>94</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>342.75</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" s="10" t="s">
         <v>95</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>368.5</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" s="10" t="s">
         <v>96</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>394.25</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" s="10" t="s">
         <v>97</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91" s="10" t="s">
         <v>98</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>-3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" s="10" t="s">
         <v>99</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93" s="10" t="s">
         <v>100</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>0.2315752168470005</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" s="10" t="s">
         <v>101</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>0.463150433694001</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A95" s="10" t="s">
         <v>102</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>-0.2315752168470005</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96" s="10" t="s">
         <v>103</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>-0.463150433694001</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A98" s="10" t="s">
         <v>104</v>
       </c>
@@ -2971,72 +2971,72 @@
         <v>0.67958533137844945</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A99" s="10" t="s">
         <v>105</v>
       </c>
       <c r="B99">
-        <f>B$67 * TAN(ASIN((B$50*B86*B$56 + B$54*SIN(RADIANS(B$58)))/B$55) - B$98)</f>
+        <f t="shared" ref="B99:C103" si="0">B$67 * TAN(ASIN((B$50*B86*B$56 + B$54*SIN(RADIANS(B$58)))/B$55) - B$98)</f>
         <v>-64.759922002707356</v>
       </c>
       <c r="C99">
-        <f>C$67 * TAN(ASIN((C$50*C86*C$56 + C$54*SIN(RADIANS(C$58)))/C$55) - C$98)</f>
+        <f t="shared" si="0"/>
         <v>-64.931254398486146</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A100" s="10" t="s">
         <v>106</v>
       </c>
       <c r="B100">
-        <f>B$67 * TAN(ASIN((B$50*B87*B$56 + B$54*SIN(RADIANS(B$58)))/B$55) - B$98)</f>
+        <f t="shared" si="0"/>
         <v>-33.020788336519892</v>
       </c>
       <c r="C100">
-        <f>C$67 * TAN(ASIN((C$50*C87*C$56 + C$54*SIN(RADIANS(C$58)))/C$55) - C$98)</f>
+        <f t="shared" si="0"/>
         <v>-33.082447813430207</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A101" s="10" t="s">
         <v>107</v>
       </c>
       <c r="B101">
-        <f>B$67 * TAN(ASIN((B$50*B88*B$56 + B$54*SIN(RADIANS(B$58)))/B$55) - B$98)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C101">
-        <f>C$67 * TAN(ASIN((C$50*C88*C$56 + C$54*SIN(RADIANS(C$58)))/C$55) - C$98)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A102" s="10" t="s">
         <v>108</v>
       </c>
       <c r="B102">
-        <f>B$67 * TAN(ASIN((B$50*B89*B$56 + B$54*SIN(RADIANS(B$58)))/B$55) - B$98)</f>
+        <f t="shared" si="0"/>
         <v>35.057157711666186</v>
       </c>
       <c r="C102">
-        <f>C$67 * TAN(ASIN((C$50*C89*C$56 + C$54*SIN(RADIANS(C$58)))/C$55) - C$98)</f>
+        <f t="shared" si="0"/>
         <v>35.03998287561857</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A103" s="10" t="s">
         <v>109</v>
       </c>
       <c r="B103">
-        <f>B$67 * TAN(ASIN((B$50*B90*B$56 + B$54*SIN(RADIANS(B$58)))/B$55) - B$98)</f>
+        <f t="shared" si="0"/>
         <v>73.250896295617295</v>
       </c>
       <c r="C103">
-        <f>C$67 * TAN(ASIN((C$50*C90*C$56 + C$54*SIN(RADIANS(C$58)))/C$55) - C$98)</f>
+        <f t="shared" si="0"/>
         <v>73.078441963971798</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A105" s="10" t="s">
         <v>110</v>
       </c>
@@ -3049,51 +3049,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A106" s="10" t="s">
         <v>111</v>
       </c>
       <c r="B106" s="15">
-        <f t="shared" ref="B106:C109" si="0">B$67 * TAN(RADIANS(B93*$B$13/B$62))</f>
+        <f t="shared" ref="B106:C109" si="1">B$67 * TAN(RADIANS(B93*$B$13/B$62))</f>
         <v>29.838455496169814</v>
       </c>
       <c r="C106" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25.309175077201669</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A107" s="10" t="s">
         <v>112</v>
       </c>
       <c r="B107" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59.913826086925553</v>
       </c>
       <c r="C107" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50.758853671139683</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A108" s="10" t="s">
         <v>113</v>
       </c>
       <c r="B108" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-29.838455496169814</v>
       </c>
       <c r="C108" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-25.309175077201669</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A109" s="10" t="s">
         <v>114</v>
       </c>
       <c r="B109" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-59.913826086925553</v>
       </c>
       <c r="C109" s="15">
@@ -3145,32 +3145,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3824768D-5964-45D6-ABF4-96D18DC36DE7}">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" style="15" customWidth="1"/>
-    <col min="4" max="4" width="77.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="15" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="15"/>
-    <col min="7" max="7" width="14.140625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="34.73046875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="20.73046875" style="15" customWidth="1"/>
+    <col min="4" max="4" width="77.86328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="9.1328125" style="15"/>
+    <col min="7" max="7" width="14.1328125" style="15" customWidth="1"/>
     <col min="8" max="8" width="14" style="15" customWidth="1"/>
-    <col min="9" max="1025" width="8.5703125" style="15" customWidth="1"/>
-    <col min="1026" max="16384" width="9.140625" style="15"/>
+    <col min="9" max="1025" width="8.59765625" style="15" customWidth="1"/>
+    <col min="1026" max="16384" width="9.1328125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.65">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3184,14 +3184,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>8</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -3233,19 +3233,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
@@ -3281,7 +3281,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" s="15" t="s">
         <v>17</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="15" t="s">
         <v>23</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>-937.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="15" t="s">
         <v>24</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="15" t="s">
         <v>25</v>
       </c>
@@ -3346,7 +3346,7 @@
         <v>0.12532783116806537</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="15" t="s">
         <v>26</v>
       </c>
@@ -3357,7 +3357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A19" s="15" t="s">
         <v>27</v>
       </c>
@@ -3367,13 +3367,13 @@
       </c>
       <c r="C19" s="15">
         <f>DEGREES(C36/2*C12)*C18</f>
-        <v>0.463150433694001</v>
+        <v>0.49039457685247162</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="15" t="s">
         <v>29</v>
       </c>
@@ -3383,10 +3383,10 @@
       </c>
       <c r="C20" s="15">
         <f>2*B13*TAN(RADIANS(C19))</f>
-        <v>129.33881713985178</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>136.94734410983583</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="15" t="s">
         <v>30</v>
       </c>
@@ -3396,10 +3396,10 @@
       </c>
       <c r="C21" s="15">
         <f>C20/2</f>
-        <v>64.669408569925892</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>68.473672054917913</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="15" t="s">
         <v>31</v>
       </c>
@@ -3408,12 +3408,12 @@
         <v>6.5024999999999995</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="15" t="s">
         <v>33</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>35</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="15" t="s">
         <v>37</v>
       </c>
@@ -3445,10 +3445,10 @@
       </c>
       <c r="C27" s="15">
         <f>C26*C20</f>
-        <v>129.33881713985178</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>136.94734410983583</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="15" t="s">
         <v>30</v>
       </c>
@@ -3458,15 +3458,15 @@
       </c>
       <c r="C28" s="15">
         <f>C27/2</f>
-        <v>64.669408569925892</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+        <v>68.473672054917913</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" s="15" t="s">
         <v>39</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" s="15" t="s">
         <v>27</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>0.11785113019775792</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A34" s="2" t="s">
         <v>40</v>
       </c>
@@ -3496,7 +3496,7 @@
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="s">
         <v>236</v>
       </c>
@@ -3507,18 +3507,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>41</v>
       </c>
       <c r="B36" s="15">
+        <f>ROUND(64*2/B41,0)</f>
         <v>64</v>
       </c>
       <c r="C36" s="15">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <f>ROUNDUP(53*2/C41,0)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>42</v>
       </c>
@@ -3529,7 +3531,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="10" t="s">
         <v>43</v>
       </c>
@@ -3539,10 +3541,10 @@
       </c>
       <c r="C38" s="17">
         <f>C42/C43</f>
-        <v>0.70106818401597426</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0.74230748895809029</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>44</v>
       </c>
@@ -3553,7 +3555,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>45</v>
       </c>
@@ -3566,7 +3568,7 @@
         <v>0.8660254037844386</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="15" t="s">
         <v>46</v>
       </c>
@@ -3579,7 +3581,7 @@
         <v>1.9918584287042087</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="10" t="s">
         <v>47</v>
       </c>
@@ -3589,10 +3591,10 @@
       </c>
       <c r="C42" s="17">
         <f>C39*C36*C40</f>
-        <v>101.58477986391465</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>107.56035515002726</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="10" t="s">
         <v>48</v>
       </c>
@@ -3606,8 +3608,8 @@
       </c>
       <c r="E43" s="8"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="33" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A44" s="31" t="s">
         <v>83</v>
       </c>
       <c r="B44" s="15">
@@ -3618,8 +3620,8 @@
       </c>
       <c r="E44" s="8"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="33" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A45" s="31" t="s">
         <v>158</v>
       </c>
       <c r="B45" s="15">
@@ -3633,8 +3635,8 @@
       </c>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="33" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A46" s="31" t="s">
         <v>158</v>
       </c>
       <c r="B46" s="15">
@@ -3648,7 +3650,7 @@
       </c>
       <c r="E46" s="8"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="15" t="s">
         <v>240</v>
       </c>
@@ -3665,7 +3667,7 @@
       </c>
       <c r="E47" s="8"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="15" t="s">
         <v>240</v>
       </c>
@@ -3682,7 +3684,7 @@
       </c>
       <c r="E48" s="8"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="15" t="s">
         <v>88</v>
       </c>
@@ -3699,7 +3701,7 @@
       </c>
       <c r="E49" s="8"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" s="15" t="s">
         <v>88</v>
       </c>
@@ -3716,7 +3718,7 @@
       </c>
       <c r="E50" s="8"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" s="12" t="s">
         <v>237</v>
       </c>
@@ -3728,7 +3730,7 @@
       </c>
       <c r="E51" s="8"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="15" t="s">
         <v>15</v>
       </c>
@@ -3742,7 +3744,7 @@
       </c>
       <c r="E52" s="8"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" s="15" t="s">
         <v>16</v>
       </c>
@@ -3756,7 +3758,7 @@
       </c>
       <c r="E53" s="8"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" s="10" t="s">
         <v>49</v>
       </c>
@@ -3770,7 +3772,7 @@
       </c>
       <c r="E54" s="8"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" s="10" t="s">
         <v>50</v>
       </c>
@@ -3784,7 +3786,7 @@
       </c>
       <c r="E55" s="8"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="10" t="s">
         <v>33</v>
       </c>
@@ -3796,7 +3798,7 @@
       </c>
       <c r="E56" s="8"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" s="9" t="s">
         <v>52</v>
       </c>
@@ -3808,8 +3810,8 @@
       </c>
       <c r="E57" s="8"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="34" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A58" s="32" t="s">
         <v>60</v>
       </c>
       <c r="B58" s="15">
@@ -3820,8 +3822,8 @@
       </c>
       <c r="E58" s="8"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="34" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A59" s="32" t="s">
         <v>142</v>
       </c>
       <c r="B59" s="23">
@@ -3832,11 +3834,11 @@
       </c>
       <c r="E59" s="8"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="34" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A60" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B60" s="35">
+      <c r="B60" s="33">
         <v>9</v>
       </c>
       <c r="C60" s="23">
@@ -3844,7 +3846,7 @@
       </c>
       <c r="E60" s="8"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" s="15" t="s">
         <v>53</v>
       </c>
@@ -3853,14 +3855,14 @@
         <v>428.25</v>
       </c>
       <c r="C61" s="17">
-        <f>ABS(C57)*C74*1000*C71</f>
-        <v>334.26536127890915</v>
+        <f>ABS(C57)*C59*1000*C58</f>
+        <v>404.7</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A62" s="10" t="s">
         <v>55</v>
       </c>
@@ -3870,14 +3872,14 @@
       </c>
       <c r="C62" s="17">
         <f>C52/C61</f>
-        <v>0.94834833853902367</v>
+        <v>0.78329626884111692</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="31" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A63" s="29" t="s">
         <v>238</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -3887,8 +3889,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="33" t="s">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A64" s="31" t="s">
         <v>84</v>
       </c>
       <c r="B64" s="17">
@@ -3898,8 +3900,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="32" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65" s="30" t="s">
         <v>235</v>
       </c>
       <c r="B65" s="17">
@@ -3914,8 +3916,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="32" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A66" s="30" t="s">
         <v>235</v>
       </c>
       <c r="B66" s="17">
@@ -3930,19 +3932,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="32"/>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A67" s="30"/>
       <c r="B67" s="17"/>
       <c r="C67" s="17"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="9" t="s">
         <v>58</v>
       </c>
@@ -3953,7 +3955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" s="9" t="s">
         <v>59</v>
       </c>
@@ -3964,7 +3966,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="9" t="s">
         <v>60</v>
       </c>
@@ -3978,7 +3980,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A72" s="9" t="s">
         <v>62</v>
       </c>
@@ -3992,7 +3994,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" s="9" t="s">
         <v>64</v>
       </c>
@@ -4006,7 +4008,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" s="15" t="s">
         <v>65</v>
       </c>
@@ -4019,7 +4021,7 @@
         <v>156.93209449714044</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" s="10" t="s">
         <v>66</v>
       </c>
@@ -4035,7 +4037,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" s="10" t="s">
         <v>66</v>
       </c>
@@ -4051,7 +4053,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" s="10" t="s">
         <v>69</v>
       </c>
@@ -4064,7 +4066,7 @@
         <v>615.1371798225174</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" s="10" t="s">
         <v>70</v>
       </c>
@@ -4077,7 +4079,7 @@
         <v>1230.2743596450348</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" s="10" t="s">
         <v>71</v>
       </c>
@@ -4093,7 +4095,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" s="10" t="s">
         <v>73</v>
       </c>
@@ -4103,10 +4105,10 @@
       </c>
       <c r="C80" s="13">
         <f>2*DEGREES(ATAN($C$28/C77))</f>
-        <v>12.002926945070323</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>12.703402539008794</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A81" s="10" t="s">
         <v>74</v>
       </c>
@@ -4116,13 +4118,13 @@
       </c>
       <c r="C81" s="13">
         <f>C80/C79</f>
-        <v>0.73523792360897067</v>
+        <v>0.77814547637364051</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A82" s="10" t="s">
         <v>76</v>
       </c>
@@ -4138,7 +4140,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" s="10" t="s">
         <v>78</v>
       </c>
@@ -4151,7 +4153,7 @@
         <v>1010.2051780808947</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A84" s="14" t="s">
         <v>79</v>
       </c>
@@ -4161,13 +4163,13 @@
       </c>
       <c r="C84" s="13">
         <f>2*C82*TAN(RADIANS(C80/2))</f>
-        <v>106.20293089684043</v>
+        <v>112.45045876116468</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" s="10" t="s">
         <v>81</v>
       </c>
@@ -4180,7 +4182,7 @@
         <v>3.7648456683463967</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A86" s="10" t="s">
         <v>82</v>
       </c>
@@ -4193,7 +4195,7 @@
         <v>4.7709937810922209</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A87" s="10" t="s">
         <v>83</v>
       </c>
@@ -4206,7 +4208,7 @@
         <v>3.2587263809061118</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A88" s="10" t="s">
         <v>84</v>
       </c>
@@ -4217,7 +4219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A89" s="10" t="s">
         <v>235</v>
       </c>
@@ -4233,7 +4235,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A90" s="10" t="s">
         <v>235</v>
       </c>
@@ -4249,7 +4251,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A91" s="10" t="s">
         <v>85</v>
       </c>
@@ -4265,7 +4267,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A92" s="10" t="s">
         <v>85</v>
       </c>
@@ -4281,7 +4283,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A93" s="10" t="s">
         <v>88</v>
       </c>
@@ -4297,7 +4299,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A94" s="10" t="s">
         <v>88</v>
       </c>
@@ -4313,7 +4315,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A95" s="10" t="s">
         <v>89</v>
       </c>
@@ -4329,7 +4331,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A96" s="10" t="s">
         <v>89</v>
       </c>
@@ -4345,7 +4347,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A97" s="10" t="s">
         <v>91</v>
       </c>
@@ -4361,7 +4363,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98" s="10" t="s">
         <v>91</v>
       </c>
@@ -4377,15 +4379,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99" s="10"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100" s="12" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A101" s="10" t="s">
         <v>93</v>
       </c>
@@ -4396,7 +4398,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A102" s="10" t="s">
         <v>94</v>
       </c>
@@ -4409,7 +4411,7 @@
         <v>342.75</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A103" s="10" t="s">
         <v>95</v>
       </c>
@@ -4422,7 +4424,7 @@
         <v>368.5</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A104" s="10" t="s">
         <v>96</v>
       </c>
@@ -4435,7 +4437,7 @@
         <v>394.25</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A105" s="10" t="s">
         <v>97</v>
       </c>
@@ -4448,7 +4450,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A106" s="10" t="s">
         <v>98</v>
       </c>
@@ -4459,7 +4461,7 @@
         <v>-3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A107" s="10" t="s">
         <v>99</v>
       </c>
@@ -4470,7 +4472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A108" s="10" t="s">
         <v>100</v>
       </c>
@@ -4480,10 +4482,10 @@
       </c>
       <c r="C108" s="13">
         <f>C109/2</f>
-        <v>0.2315752168470005</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.24519728842623581</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A109" s="10" t="s">
         <v>101</v>
       </c>
@@ -4493,10 +4495,10 @@
       </c>
       <c r="C109" s="13">
         <f>C19</f>
-        <v>0.463150433694001</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.49039457685247162</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A110" s="10" t="s">
         <v>102</v>
       </c>
@@ -4506,10 +4508,10 @@
       </c>
       <c r="C110" s="13">
         <f>C111/2</f>
-        <v>-0.2315752168470005</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-0.24519728842623581</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A111" s="10" t="s">
         <v>103</v>
       </c>
@@ -4519,10 +4521,10 @@
       </c>
       <c r="C111" s="13">
         <f>-C19</f>
-        <v>-0.463150433694001</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>-0.49039457685247162</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A113" s="10" t="s">
         <v>104</v>
       </c>
@@ -4538,87 +4540,87 @@
       <c r="F113" s="15"/>
       <c r="G113" s="15"/>
     </row>
-    <row r="114" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A114" s="10" t="s">
         <v>105</v>
       </c>
       <c r="B114" s="15">
-        <f>B$82 * TAN(ASIN((B$57*B101*B$71 + B$69*SIN(RADIANS(B$73)))/B$70) - B$113)</f>
+        <f t="shared" ref="B114:C118" si="0">B$82 * TAN(ASIN((B$57*B101*B$71 + B$69*SIN(RADIANS(B$73)))/B$70) - B$113)</f>
         <v>-67.997918102842718</v>
       </c>
       <c r="C114" s="15">
-        <f>C$82 * TAN(ASIN((C$57*C101*C$71 + C$69*SIN(RADIANS(C$73)))/C$70) - C$113)</f>
+        <f t="shared" si="0"/>
         <v>-68.177817118410445</v>
       </c>
       <c r="E114" s="15"/>
       <c r="F114" s="15"/>
       <c r="G114" s="15"/>
     </row>
-    <row r="115" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A115" s="10" t="s">
         <v>106</v>
       </c>
       <c r="B115" s="15">
-        <f>B$82 * TAN(ASIN((B$57*B102*B$71 + B$69*SIN(RADIANS(B$73)))/B$70) - B$113)</f>
+        <f t="shared" si="0"/>
         <v>-34.67182775334588</v>
       </c>
       <c r="C115" s="15">
-        <f>C$82 * TAN(ASIN((C$57*C102*C$71 + C$69*SIN(RADIANS(C$73)))/C$70) - C$113)</f>
+        <f t="shared" si="0"/>
         <v>-34.736570204101717</v>
       </c>
       <c r="E115" s="15"/>
       <c r="F115" s="15"/>
       <c r="G115" s="15"/>
     </row>
-    <row r="116" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A116" s="10" t="s">
         <v>107</v>
       </c>
       <c r="B116" s="15">
-        <f>B$82 * TAN(ASIN((B$57*B103*B$71 + B$69*SIN(RADIANS(B$73)))/B$70) - B$113)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C116" s="15">
-        <f>C$82 * TAN(ASIN((C$57*C103*C$71 + C$69*SIN(RADIANS(C$73)))/C$70) - C$113)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E116" s="15"/>
       <c r="F116" s="15"/>
       <c r="G116" s="15"/>
     </row>
-    <row r="117" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A117" s="10" t="s">
         <v>108</v>
       </c>
       <c r="B117" s="15">
-        <f>B$82 * TAN(ASIN((B$57*B104*B$71 + B$69*SIN(RADIANS(B$73)))/B$70) - B$113)</f>
+        <f t="shared" si="0"/>
         <v>36.810015597249489</v>
       </c>
       <c r="C117" s="15">
-        <f>C$82 * TAN(ASIN((C$57*C104*C$71 + C$69*SIN(RADIANS(C$73)))/C$70) - C$113)</f>
+        <f t="shared" si="0"/>
         <v>36.791982019399491</v>
       </c>
       <c r="E117" s="15"/>
       <c r="F117" s="15"/>
       <c r="G117" s="15"/>
     </row>
-    <row r="118" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A118" s="10" t="s">
         <v>109</v>
       </c>
       <c r="B118" s="15">
-        <f>B$82 * TAN(ASIN((B$57*B105*B$71 + B$69*SIN(RADIANS(B$73)))/B$70) - B$113)</f>
+        <f t="shared" si="0"/>
         <v>76.913441110398153</v>
       </c>
       <c r="C118" s="15">
-        <f>C$82 * TAN(ASIN((C$57*C105*C$71 + C$69*SIN(RADIANS(C$73)))/C$70) - C$113)</f>
+        <f t="shared" si="0"/>
         <v>76.732364062170376</v>
       </c>
       <c r="E118" s="15"/>
       <c r="F118" s="15"/>
       <c r="G118" s="15"/>
     </row>
-    <row r="120" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A120" s="10" t="s">
         <v>110</v>
       </c>
@@ -4634,65 +4636,65 @@
       <c r="F120" s="15"/>
       <c r="G120" s="15"/>
     </row>
-    <row r="121" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A121" s="10" t="s">
         <v>111</v>
       </c>
       <c r="B121" s="15">
-        <f>B$82 * TAN(RADIANS(B108*$B$13/B$77))</f>
+        <f t="shared" ref="B121:C124" si="1">B$82 * TAN(RADIANS(B108*$B$13/B$77))</f>
         <v>33.425135696144217</v>
       </c>
       <c r="C121" s="15">
-        <f>C$82 * TAN(RADIANS(C108*$B$13/C$77))</f>
-        <v>26.57463383106175</v>
+        <f t="shared" si="1"/>
+        <v>28.140990504882957</v>
       </c>
       <c r="E121" s="15"/>
       <c r="F121" s="15"/>
       <c r="G121" s="15"/>
     </row>
-    <row r="122" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A122" s="10" t="s">
         <v>112</v>
       </c>
       <c r="B122" s="15">
-        <f>B$82 * TAN(RADIANS(B109*$B$13/B$77))</f>
+        <f t="shared" si="1"/>
         <v>67.152505154646747</v>
       </c>
       <c r="C122" s="15">
-        <f>C$82 * TAN(RADIANS(C109*$B$13/C$77))</f>
-        <v>53.296796354696653</v>
+        <f t="shared" si="1"/>
+        <v>56.457223366558978</v>
       </c>
       <c r="E122" s="15"/>
       <c r="F122" s="15"/>
       <c r="G122" s="15"/>
     </row>
-    <row r="123" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A123" s="10" t="s">
         <v>113</v>
       </c>
       <c r="B123" s="15">
-        <f>B$82 * TAN(RADIANS(B110*$B$13/B$77))</f>
+        <f t="shared" si="1"/>
         <v>-33.425135696144217</v>
       </c>
       <c r="C123" s="15">
-        <f>C$82 * TAN(RADIANS(C110*$B$13/C$77))</f>
-        <v>-26.57463383106175</v>
+        <f t="shared" si="1"/>
+        <v>-28.140990504882957</v>
       </c>
       <c r="E123" s="15"/>
       <c r="F123" s="15"/>
       <c r="G123" s="15"/>
     </row>
-    <row r="124" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A124" s="10" t="s">
         <v>114</v>
       </c>
       <c r="B124" s="15">
-        <f>B$82 * TAN(RADIANS(B111*$B$13/B$77))</f>
+        <f t="shared" si="1"/>
         <v>-67.152505154646747</v>
       </c>
       <c r="C124" s="15">
-        <f>C$82 * TAN(RADIANS(C111*$B$13/C$77))</f>
-        <v>-53.296796354696653</v>
+        <f t="shared" si="1"/>
+        <v>-56.457223366558978</v>
       </c>
       <c r="E124" s="15"/>
       <c r="F124" s="15"/>
@@ -4746,30 +4748,30 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" customWidth="1"/>
+    <col min="3" max="3" width="15.265625" customWidth="1"/>
+    <col min="4" max="4" width="17.265625" customWidth="1"/>
+    <col min="5" max="5" width="19.73046875" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="10" width="8.5703125" customWidth="1"/>
+    <col min="7" max="10" width="8.59765625" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125"/>
-    <col min="16" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="8.59765625" customWidth="1"/>
+    <col min="13" max="13" width="10.73046875" customWidth="1"/>
+    <col min="14" max="14" width="19.1328125" customWidth="1"/>
+    <col min="15" max="15" width="11.3984375"/>
+    <col min="16" max="1025" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>115</v>
       </c>
       <c r="B2" s="4"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -4810,7 +4812,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4">
         <f>'Spectrometer Design'!B13</f>
         <v>8000</v>
@@ -4863,7 +4865,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>8000</v>
       </c>
@@ -4914,7 +4916,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>8000</v>
       </c>
@@ -4965,7 +4967,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>16000</v>
       </c>
@@ -5017,7 +5019,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>9698.82</v>
       </c>
@@ -5081,27 +5083,27 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="77.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="34.73046875" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" customWidth="1"/>
+    <col min="3" max="3" width="13.73046875" customWidth="1"/>
+    <col min="4" max="4" width="77.86328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" customWidth="1"/>
+    <col min="6" max="6" width="11.3984375"/>
+    <col min="7" max="7" width="14.1328125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="9" max="1025" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.65">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -5111,14 +5113,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -5130,7 +5132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -5143,7 +5145,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -5155,19 +5157,19 @@
         <v>132</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
       <c r="B7" s="18"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -5178,7 +5180,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -5186,7 +5188,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
@@ -5194,7 +5196,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -5206,7 +5208,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -5218,7 +5220,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
@@ -5229,7 +5231,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
@@ -5240,7 +5242,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -5249,7 +5251,7 @@
         <v>-937.5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -5258,7 +5260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -5267,7 +5269,7 @@
         <v>0.1001674211615598</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -5283,7 +5285,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -5292,7 +5294,7 @@
         <v>78.85275439069963</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -5301,7 +5303,7 @@
         <v>39.426377195349815</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -5310,12 +5312,12 @@
         <v>5.4931640625</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A24" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -5323,7 +5325,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>35</v>
       </c>
@@ -5334,7 +5336,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -5343,7 +5345,7 @@
         <v>78.85275439069963</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -5352,7 +5354,7 @@
         <v>39.426377195349815</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
@@ -5365,12 +5367,12 @@
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -5381,7 +5383,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>42</v>
       </c>
@@ -5392,7 +5394,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="10" t="s">
         <v>43</v>
       </c>
@@ -5401,7 +5403,7 @@
         <v>0.30070326520293006</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -5412,7 +5414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -5425,7 +5427,7 @@
         <v>0.8660254037844386</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -5438,7 +5440,7 @@
         <v>1.7320508075688772</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="10" t="s">
         <v>47</v>
       </c>
@@ -5451,7 +5453,7 @@
         <v>43.301270189221931</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" s="10" t="s">
         <v>48</v>
       </c>
@@ -5465,13 +5467,13 @@
       </c>
       <c r="E39" s="8"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="8"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>15</v>
       </c>
@@ -5483,7 +5485,7 @@
       </c>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="9" t="s">
         <v>16</v>
       </c>
@@ -5495,7 +5497,7 @@
       </c>
       <c r="E42" s="8"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="10" t="s">
         <v>49</v>
       </c>
@@ -5509,7 +5511,7 @@
       </c>
       <c r="E43" s="8"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" s="10" t="s">
         <v>50</v>
       </c>
@@ -5523,7 +5525,7 @@
       </c>
       <c r="E44" s="8"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" s="10" t="s">
         <v>33</v>
       </c>
@@ -5535,7 +5537,7 @@
       </c>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" s="9" t="s">
         <v>52</v>
       </c>
@@ -5547,7 +5549,7 @@
       </c>
       <c r="E46" s="8"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>137</v>
       </c>
@@ -5560,7 +5562,7 @@
         <v>257.59223300970871</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="10" t="s">
         <v>138</v>
       </c>
@@ -5573,7 +5575,7 @@
         <v>1.2306271671943316</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
         <v>139</v>
       </c>
@@ -5584,7 +5586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>83</v>
       </c>
@@ -5600,10 +5602,10 @@
         <v>140</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="10"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" s="12" t="s">
         <v>57</v>
       </c>
@@ -5614,7 +5616,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" s="9" t="s">
         <v>58</v>
       </c>
@@ -5625,7 +5627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" s="9" t="s">
         <v>59</v>
       </c>
@@ -5636,7 +5638,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A55" s="9" t="s">
         <v>141</v>
       </c>
@@ -5650,7 +5652,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="9" t="s">
         <v>64</v>
       </c>
@@ -5664,7 +5666,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>142</v>
       </c>
@@ -5680,7 +5682,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A58" s="10" t="s">
         <v>66</v>
       </c>
@@ -5696,7 +5698,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" s="10" t="s">
         <v>66</v>
       </c>
@@ -5712,7 +5714,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" s="10" t="s">
         <v>66</v>
       </c>
@@ -5728,7 +5730,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" s="10" t="s">
         <v>76</v>
       </c>
@@ -5741,7 +5743,7 @@
         <v>618.58957413174187</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="10" t="s">
         <v>78</v>
       </c>
@@ -5754,7 +5756,7 @@
         <v>1237.1791482634837</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="10" t="s">
         <v>147</v>
       </c>
@@ -5767,7 +5769,7 @@
         <v>2.0045340321059042</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" s="10" t="s">
         <v>148</v>
       </c>
@@ -5780,7 +5782,7 @@
         <v>6.6390012002412089</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="10" t="s">
         <v>69</v>
       </c>
@@ -5793,7 +5795,7 @@
         <v>1492.48115565993</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="10" t="s">
         <v>70</v>
       </c>
@@ -5806,7 +5808,7 @@
         <v>2984.96231131986</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="10" t="s">
         <v>60</v>
       </c>
@@ -5820,7 +5822,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="10" t="s">
         <v>150</v>
       </c>
@@ -5836,7 +5838,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="10" t="s">
         <v>151</v>
       </c>
@@ -5852,7 +5854,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A70" s="10" t="s">
         <v>53</v>
       </c>
@@ -5868,10 +5870,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="10"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" s="11" t="s">
         <v>154</v>
       </c>
@@ -5882,7 +5884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A73" s="14" t="s">
         <v>79</v>
       </c>
@@ -5898,7 +5900,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A74" s="14" t="s">
         <v>156</v>
       </c>
@@ -5914,7 +5916,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A75" s="10" t="s">
         <v>158</v>
       </c>
@@ -5930,7 +5932,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A76" s="10" t="s">
         <v>158</v>
       </c>
@@ -5946,7 +5948,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" s="10" t="s">
         <v>83</v>
       </c>
@@ -5962,7 +5964,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" s="10" t="s">
         <v>85</v>
       </c>
@@ -5978,7 +5980,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" s="10" t="s">
         <v>85</v>
       </c>
@@ -5994,7 +5996,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" s="10" t="s">
         <v>88</v>
       </c>
@@ -6010,7 +6012,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A81" s="10" t="s">
         <v>88</v>
       </c>
@@ -6026,7 +6028,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A82" s="10" t="s">
         <v>89</v>
       </c>
@@ -6042,7 +6044,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A83" s="10" t="s">
         <v>89</v>
       </c>
@@ -6058,7 +6060,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A84" s="10" t="s">
         <v>91</v>
       </c>
@@ -6074,7 +6076,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A85" s="10" t="s">
         <v>91</v>
       </c>
@@ -6177,27 +6179,27 @@
       <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="77.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="34.73046875" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" customWidth="1"/>
+    <col min="3" max="3" width="20.73046875" customWidth="1"/>
+    <col min="4" max="4" width="77.86328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" customWidth="1"/>
+    <col min="6" max="6" width="11.3984375"/>
+    <col min="7" max="7" width="14.1328125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="9" max="1025" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.65">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -6211,14 +6213,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -6232,7 +6234,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -6248,7 +6250,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -6262,19 +6264,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -6288,7 +6290,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -6299,7 +6301,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
@@ -6310,7 +6312,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -6326,7 +6328,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
@@ -6337,7 +6339,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -6348,7 +6350,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -6357,7 +6359,7 @@
         <v>-937.5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -6366,7 +6368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -6375,7 +6377,7 @@
         <v>0.1001674211615598</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -6391,7 +6393,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -6404,7 +6406,7 @@
         <v>90.300613600275852</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -6417,7 +6419,7 @@
         <v>45.150306800137926</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -6426,12 +6428,12 @@
         <v>5.4931640625</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A23" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -6439,7 +6441,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
@@ -6450,7 +6452,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -6459,7 +6461,7 @@
         <v>90.34561451808068</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>30</v>
       </c>
@@ -6468,7 +6470,7 @@
         <v>45.17280725904034</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="18" x14ac:dyDescent="0.45">
       <c r="A29" s="2" t="s">
         <v>40</v>
       </c>
@@ -6481,12 +6483,12 @@
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="9" t="s">
         <v>41</v>
       </c>
@@ -6497,7 +6499,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>42</v>
       </c>
@@ -6508,7 +6510,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" s="10" t="s">
         <v>43</v>
       </c>
@@ -6521,7 +6523,7 @@
         <v>0.25860480807451985</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>44</v>
       </c>
@@ -6532,7 +6534,7 @@
         <v>3.05</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>45</v>
       </c>
@@ -6545,7 +6547,7 @@
         <v>0.8660254037844386</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -6558,7 +6560,7 @@
         <v>2.6413774815425377</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" s="10" t="s">
         <v>47</v>
       </c>
@@ -6571,7 +6573,7 @@
         <v>56.789615853164563</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" s="10" t="s">
         <v>48</v>
       </c>
@@ -6585,13 +6587,13 @@
       </c>
       <c r="E38" s="8"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E39" s="8"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>15</v>
       </c>
@@ -6605,7 +6607,7 @@
       </c>
       <c r="E40" s="8"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>16</v>
       </c>
@@ -6619,7 +6621,7 @@
       </c>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" s="10" t="s">
         <v>49</v>
       </c>
@@ -6633,7 +6635,7 @@
       </c>
       <c r="E42" s="8"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" s="10" t="s">
         <v>50</v>
       </c>
@@ -6647,7 +6649,7 @@
       </c>
       <c r="E43" s="8"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" s="10" t="s">
         <v>33</v>
       </c>
@@ -6659,7 +6661,7 @@
       </c>
       <c r="E44" s="8"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" s="9" t="s">
         <v>52</v>
       </c>
@@ -6671,7 +6673,7 @@
       </c>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>53</v>
       </c>
@@ -6687,7 +6689,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A47" s="10" t="s">
         <v>55</v>
       </c>
@@ -6703,12 +6705,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" s="9" t="s">
         <v>58</v>
       </c>
@@ -6719,7 +6721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" s="9" t="s">
         <v>59</v>
       </c>
@@ -6730,7 +6732,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" s="9" t="s">
         <v>60</v>
       </c>
@@ -6744,7 +6746,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A52" s="9" t="s">
         <v>62</v>
       </c>
@@ -6758,7 +6760,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" s="9" t="s">
         <v>64</v>
       </c>
@@ -6772,7 +6774,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>65</v>
       </c>
@@ -6785,7 +6787,7 @@
         <v>128.28801347417394</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" s="10" t="s">
         <v>66</v>
       </c>
@@ -6798,7 +6800,7 @@
         <v>38.143630623771593</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" s="10" t="s">
         <v>66</v>
       </c>
@@ -6811,7 +6813,7 @@
         <v>63.050831780852853</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" s="10" t="s">
         <v>69</v>
       </c>
@@ -6824,7 +6826,7 @@
         <v>621.86714819163751</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" s="10" t="s">
         <v>70</v>
       </c>
@@ -6837,7 +6839,7 @@
         <v>1243.734296383275</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" s="10" t="s">
         <v>71</v>
       </c>
@@ -6853,7 +6855,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" s="10" t="s">
         <v>73</v>
       </c>
@@ -6866,7 +6868,7 @@
         <v>8.3094056426406713</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A61" s="10" t="s">
         <v>74</v>
       </c>
@@ -6882,7 +6884,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" s="10" t="s">
         <v>76</v>
       </c>
@@ -6898,7 +6900,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" s="10" t="s">
         <v>78</v>
       </c>
@@ -6911,7 +6913,7 @@
         <v>994.36170333796406</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A64" s="14" t="s">
         <v>79</v>
       </c>
@@ -6927,7 +6929,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" s="10" t="s">
         <v>81</v>
       </c>
@@ -6940,7 +6942,7 @@
         <v>4.9277532915231186</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" s="10" t="s">
         <v>82</v>
       </c>
@@ -6953,7 +6955,7 @@
         <v>8.5514265429060892</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" s="10" t="s">
         <v>83</v>
       </c>
@@ -6966,7 +6968,7 @@
         <v>3.9774468133518561</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" s="10" t="s">
         <v>85</v>
       </c>
@@ -6982,7 +6984,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" s="10" t="s">
         <v>85</v>
       </c>
@@ -6998,7 +7000,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" s="10" t="s">
         <v>88</v>
       </c>
@@ -7014,7 +7016,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" s="10" t="s">
         <v>88</v>
       </c>
@@ -7030,7 +7032,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A72" s="10" t="s">
         <v>89</v>
       </c>
@@ -7046,7 +7048,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" s="10" t="s">
         <v>89</v>
       </c>
@@ -7062,7 +7064,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" s="10" t="s">
         <v>91</v>
       </c>
@@ -7078,7 +7080,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" s="10" t="s">
         <v>91</v>
       </c>
@@ -7142,16 +7144,16 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="46.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="5" width="11.140625" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="46.59765625" customWidth="1"/>
+    <col min="2" max="2" width="12.73046875" customWidth="1"/>
+    <col min="3" max="5" width="11.1328125" customWidth="1"/>
+    <col min="6" max="6" width="12.73046875" customWidth="1"/>
+    <col min="7" max="1025" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>163</v>
       </c>
@@ -7180,7 +7182,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>170</v>
       </c>
@@ -7217,7 +7219,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -7249,7 +7251,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -7286,7 +7288,7 @@
         <v>1.63048394391678</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="24" t="s">
         <v>52</v>
       </c>
@@ -7319,7 +7321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="24" t="s">
         <v>172</v>
       </c>
@@ -7354,7 +7356,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="24" t="s">
         <v>173</v>
       </c>
@@ -7389,7 +7391,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>174</v>
       </c>
@@ -7426,7 +7428,7 @@
         <v>-66.632514973334494</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>175</v>
       </c>
@@ -7463,7 +7465,7 @@
         <v>-46.632514973334494</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>176</v>
       </c>
@@ -7500,7 +7502,7 @@
         <v>911.10928340018359</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="24" t="s">
         <v>35</v>
       </c>
@@ -7535,7 +7537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -7572,7 +7574,7 @@
         <v>875.8300154897787</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -7609,12 +7611,12 @@
         <v>2.2795115332428773</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="24" t="s">
         <v>178</v>
       </c>
@@ -7649,7 +7651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="25" t="s">
         <v>142</v>
       </c>
@@ -7686,7 +7688,7 @@
         <v>291.9433384965929</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="25" t="s">
         <v>179</v>
       </c>
@@ -7723,7 +7725,7 @@
         <v>7.8684577804757119</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" s="25" t="s">
         <v>25</v>
       </c>
@@ -7760,7 +7762,7 @@
         <v>6.3544853890004721E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" s="25" t="s">
         <v>180</v>
       </c>
@@ -7797,7 +7799,7 @@
         <v>3.643306662794592</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" s="25" t="s">
         <v>181</v>
       </c>
@@ -7834,7 +7836,7 @@
         <v>2.4250916267360467</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" s="25" t="s">
         <v>182</v>
       </c>
@@ -7885,28 +7887,28 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.86328125" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" customWidth="1"/>
+    <col min="3" max="3" width="20.73046875" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" customWidth="1"/>
+    <col min="6" max="6" width="11.3984375"/>
+    <col min="7" max="7" width="14.1328125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="9" max="1025" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.65">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
       <c r="D1" s="26"/>
     </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.65">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -7916,7 +7918,7 @@
       </c>
       <c r="D2" s="26"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -7924,7 +7926,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -7933,7 +7935,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -7941,7 +7943,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -7950,7 +7952,7 @@
         <v>27.562393169224144</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>184</v>
       </c>
@@ -7961,7 +7963,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>184</v>
       </c>
@@ -7972,7 +7974,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>185</v>
       </c>
@@ -7980,7 +7982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -7988,23 +7990,23 @@
         <v>800</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="35"/>
       <c r="D12">
         <v>1.5</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="G12" s="30"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="35"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="10" t="s">
         <v>189</v>
       </c>
@@ -8027,7 +8029,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="10" t="s">
         <v>193</v>
       </c>
@@ -8052,7 +8054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="10" t="s">
         <v>194</v>
       </c>
@@ -8077,7 +8079,7 @@
         <v>18.027883056026159</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="10" t="s">
         <v>116</v>
       </c>
@@ -8103,7 +8105,7 @@
         <v>36.055934991275898</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="10" t="s">
         <v>195</v>
       </c>
@@ -8131,7 +8133,7 @@
         <v>-18.027883056026159</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="10" t="s">
         <v>197</v>
       </c>
@@ -8164,7 +8166,7 @@
         <v>-36.055934991275898</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="10" t="s">
         <v>198</v>
       </c>
@@ -8185,13 +8187,13 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="11" t="s">
         <v>199</v>
       </c>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="10" t="s">
         <v>24</v>
       </c>
@@ -8203,7 +8205,7 @@
       </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="10" t="s">
         <v>116</v>
       </c>
@@ -8219,7 +8221,7 @@
         <v>4.0549999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="10" t="s">
         <v>200</v>
       </c>
@@ -8236,16 +8238,16 @@
         <v>8.5977802354563371E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="10"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A25" s="27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="18" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
       <c r="B26" t="s">
         <v>201</v>
@@ -8254,7 +8256,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>203</v>
       </c>
@@ -8265,12 +8267,12 @@
         <v>669</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="10" t="s">
         <v>205</v>
       </c>
@@ -8281,7 +8283,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="10" t="s">
         <v>206</v>
       </c>
@@ -8292,7 +8294,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="10" t="s">
         <v>207</v>
       </c>
@@ -8303,7 +8305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="10" t="s">
         <v>208</v>
       </c>
@@ -8314,7 +8316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="10" t="s">
         <v>209</v>
       </c>
@@ -8325,7 +8327,7 @@
         <v>75.263999999999996</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="10" t="s">
         <v>210</v>
       </c>
@@ -8338,7 +8340,7 @@
         <v>489.21599999999995</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="10" t="s">
         <v>173</v>
       </c>
@@ -8349,7 +8351,7 @@
         <v>3.2499999999999999E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="10" t="s">
         <v>211</v>
       </c>
@@ -8362,7 +8364,7 @@
         <v>153.84615384615387</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="10" t="s">
         <v>212</v>
       </c>
@@ -8373,7 +8375,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="10" t="s">
         <v>213</v>
       </c>
@@ -8386,12 +8388,12 @@
         <v>25.146079373933173</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="10" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="10" t="s">
         <v>215</v>
       </c>
@@ -8402,7 +8404,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="10" t="s">
         <v>216</v>
       </c>
@@ -8415,7 +8417,7 @@
         <v>-52.318745434843741</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="10" t="s">
         <v>156</v>
       </c>
@@ -8428,7 +8430,7 @@
         <v>144.97111081477917</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="10" t="s">
         <v>217</v>
       </c>
@@ -8441,7 +8443,7 @@
         <v>4.0526980308760416</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" s="10" t="s">
         <v>218</v>
       </c>
@@ -8454,12 +8456,12 @@
         <v>420</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" s="10" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" s="10" t="s">
         <v>220</v>
       </c>
@@ -8472,7 +8474,7 @@
         <v>27.562393169224144</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" s="10" t="s">
         <v>221</v>
       </c>
@@ -8485,27 +8487,27 @@
         <v>2.2189999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.45">
       <c r="A48" s="27" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>226</v>
       </c>
@@ -8518,12 +8520,12 @@
         <v>489.21599999999995</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>228</v>
       </c>
@@ -8531,7 +8533,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>229</v>
       </c>
@@ -8539,7 +8541,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="18" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>231</v>
       </c>
@@ -8550,7 +8552,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>234</v>
       </c>

</xml_diff>